<commit_message>
continuando la modificacion de esquemas y haciendolos mas eficientes
</commit_message>
<xml_diff>
--- a/doc/schemas.xlsx
+++ b/doc/schemas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9080" yWindow="2420" windowWidth="25240" windowHeight="17440" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
+    <workbookView xWindow="0" yWindow="1840" windowWidth="31120" windowHeight="17440" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Schemas" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="297">
   <si>
     <t>Collections</t>
   </si>
@@ -577,12 +577,6 @@
     <t>cuándo</t>
   </si>
   <si>
-    <t>[Date]</t>
-  </si>
-  <si>
-    <t>Este es un arreglo de nombres de usuario y fechas para indicar quién y cuándo realizó modificaciones. Puede ir en cualquier esquema.</t>
-  </si>
-  <si>
     <t>x.owner.user</t>
   </si>
   <si>
@@ -628,9 +622,6 @@
     <t>{permissions}</t>
   </si>
   <si>
-    <t>{modified}</t>
-  </si>
-  <si>
     <t>User.modified</t>
   </si>
   <si>
@@ -643,12 +634,6 @@
     <t>x.modified.when[]</t>
   </si>
   <si>
-    <t>quién(es) lo modificó(aron)</t>
-  </si>
-  <si>
-    <t>cuándo lo modificó(aron)</t>
-  </si>
-  <si>
     <t>read: owner, ou, mod: owner</t>
   </si>
   <si>
@@ -920,6 +905,18 @@
   </si>
   <si>
     <t>Palabras clave para búsquedas del bloque</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>quién lo modificó</t>
+  </si>
+  <si>
+    <t>cuándo lo modificó</t>
+  </si>
+  <si>
+    <t>[{modified}]</t>
   </si>
 </sst>
 </file>
@@ -1054,9 +1051,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1081,6 +1075,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1403,7 +1400,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
+      <selection pane="bottomLeft" activeCell="B88" sqref="B88:C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1448,10 +1445,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="17"/>
       <c r="C3" t="s">
         <v>13</v>
       </c>
@@ -1491,10 +1488,10 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="17"/>
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -1573,10 +1570,10 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="17"/>
       <c r="C12" t="s">
         <v>13</v>
       </c>
@@ -1590,10 +1587,10 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="17"/>
       <c r="C14" t="s">
         <v>141</v>
       </c>
@@ -1603,57 +1600,58 @@
         <v>179</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
         <v>155</v>
       </c>
       <c r="G15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H15" t="s">
-        <v>205</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
+        <v>294</v>
+      </c>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>180</v>
       </c>
       <c r="C16" t="s">
-        <v>183</v>
+        <v>293</v>
       </c>
       <c r="F16" t="s">
         <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H16" t="s">
-        <v>206</v>
-      </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
+        <v>295</v>
+      </c>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
+      <c r="B17" s="17"/>
+      <c r="C17" t="s">
+        <v>141</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
@@ -1663,16 +1661,16 @@
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H18" t="s">
-        <v>188</v>
-      </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
+        <v>186</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
@@ -1682,16 +1680,16 @@
         <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H19" t="s">
-        <v>189</v>
-      </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
+        <v>187</v>
+      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
@@ -1701,22 +1699,22 @@
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H20" t="s">
-        <v>190</v>
-      </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
+        <v>188</v>
+      </c>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="17"/>
       <c r="C21" t="s">
         <v>13</v>
       </c>
@@ -1815,7 +1813,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C28" t="s">
@@ -1832,7 +1830,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C29" t="s">
@@ -1849,24 +1847,24 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B30" s="5" t="s">
-        <v>214</v>
+      <c r="B30" s="4" t="s">
+        <v>209</v>
       </c>
       <c r="C30" t="s">
-        <v>200</v>
+        <v>296</v>
       </c>
       <c r="G30" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H30" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="17"/>
       <c r="C31" t="s">
         <v>141</v>
       </c>
@@ -1888,7 +1886,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H32" t="s">
         <v>157</v>
@@ -1914,15 +1912,15 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H33" t="s">
         <v>158</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J33" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="K33" s="4" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1943,28 +1941,28 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H34" t="s">
         <v>159</v>
       </c>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5" t="s">
+      <c r="J34" s="4"/>
+      <c r="K34" s="4" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="17"/>
       <c r="C35" t="s">
         <v>141</v>
       </c>
-      <c r="J35" s="7" t="s">
+      <c r="J35" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K35" s="7" t="s">
+      <c r="K35" s="6" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1984,8 +1982,8 @@
       <c r="H36" t="s">
         <v>160</v>
       </c>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7" t="s">
+      <c r="J36" s="6"/>
+      <c r="K36" s="6" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2005,10 +2003,10 @@
       <c r="H37" t="s">
         <v>161</v>
       </c>
-      <c r="J37" s="8" t="s">
+      <c r="J37" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K37" s="8" t="s">
+      <c r="K37" s="7" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2028,8 +2026,8 @@
       <c r="H38" t="s">
         <v>163</v>
       </c>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8" t="s">
+      <c r="J38" s="7"/>
+      <c r="K38" s="7" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2049,23 +2047,23 @@
       <c r="H39" t="s">
         <v>162</v>
       </c>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8" t="s">
+      <c r="J39" s="7"/>
+      <c r="K39" s="7" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="17"/>
       <c r="C40" t="s">
         <v>23</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="J40" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="K40" s="9"/>
+      <c r="K40" s="8"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
@@ -2083,10 +2081,10 @@
       <c r="H41" t="s">
         <v>172</v>
       </c>
-      <c r="J41" s="10" t="s">
+      <c r="J41" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="K41" s="9"/>
+      <c r="K41" s="8"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
@@ -2104,8 +2102,8 @@
       <c r="H42" t="s">
         <v>173</v>
       </c>
-      <c r="J42" s="10"/>
-      <c r="K42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="8"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
@@ -2115,13 +2113,13 @@
         <v>20</v>
       </c>
       <c r="G43" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H43" t="s">
         <v>174</v>
       </c>
-      <c r="J43" s="10"/>
-      <c r="K43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="8"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
@@ -2131,19 +2129,19 @@
         <v>20</v>
       </c>
       <c r="G44" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H44" t="s">
         <v>175</v>
       </c>
-      <c r="J44" s="10"/>
-      <c r="K44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="8"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G45" t="s">
@@ -2152,58 +2150,58 @@
       <c r="H45" t="s">
         <v>176</v>
       </c>
-      <c r="J45" s="10"/>
-      <c r="K45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="8"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>198</v>
+      <c r="B46" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="F46" t="s">
         <v>83</v>
       </c>
       <c r="G46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H46" t="s">
-        <v>208</v>
-      </c>
-      <c r="J46" s="10"/>
-      <c r="K46" s="9"/>
+        <v>203</v>
+      </c>
+      <c r="J46" s="9"/>
+      <c r="K46" s="8"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B47" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C47" t="s">
-        <v>200</v>
+      <c r="B47" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="G47" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>199</v>
+      <c r="C48" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="F48" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G48" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="B49" s="2"/>
+      <c r="B49" s="17"/>
       <c r="C49" t="s">
         <v>13</v>
       </c>
@@ -2216,10 +2214,10 @@
         <v>3</v>
       </c>
       <c r="G50" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H50" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2230,100 +2228,100 @@
         <v>72</v>
       </c>
       <c r="G51" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H51" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G52" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H52" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G53" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H53" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G54" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H54" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>198</v>
+      <c r="B55" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="F55" t="s">
         <v>83</v>
       </c>
       <c r="G55" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H55" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C56" t="s">
-        <v>200</v>
+      <c r="B56" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="G56" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H56" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>199</v>
+      <c r="C57" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="F57" t="s">
+        <v>202</v>
+      </c>
+      <c r="G57" t="s">
         <v>207</v>
       </c>
-      <c r="G57" t="s">
-        <v>212</v>
-      </c>
       <c r="H57" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2346,10 +2344,10 @@
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H59" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2363,10 +2361,10 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H60" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -2380,10 +2378,10 @@
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H61" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2397,10 +2395,10 @@
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H62" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2411,10 +2409,10 @@
         <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H63" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2425,10 +2423,10 @@
         <v>20</v>
       </c>
       <c r="G64" t="s">
-        <v>220</v>
-      </c>
-      <c r="H64" s="16" t="s">
-        <v>289</v>
+        <v>215</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2439,10 +2437,10 @@
         <v>20</v>
       </c>
       <c r="G65" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H65" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2450,13 +2448,13 @@
         <v>164</v>
       </c>
       <c r="C66" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G66" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H66" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2467,107 +2465,107 @@
         <v>3</v>
       </c>
       <c r="G67" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H67" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C68" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G68" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H68" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B69" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G69" t="s">
+        <v>223</v>
+      </c>
+      <c r="H69" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B70" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" t="s">
+        <v>224</v>
+      </c>
+      <c r="H70" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G69" t="s">
-        <v>228</v>
-      </c>
-      <c r="H69" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B70" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G70" t="s">
-        <v>229</v>
-      </c>
-      <c r="H70" t="s">
-        <v>297</v>
-      </c>
-    </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B71" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>198</v>
+      <c r="B71" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="F71" t="s">
         <v>83</v>
       </c>
       <c r="G71" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H71" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B72" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C72" t="s">
-        <v>200</v>
+      <c r="B72" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="G72" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H72" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C73" s="8" t="s">
-        <v>199</v>
+      <c r="C73" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="F73" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G73" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="H73" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B74" s="2"/>
+      <c r="B74" s="17"/>
       <c r="C74" t="s">
         <v>13</v>
       </c>
@@ -2583,10 +2581,10 @@
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H75" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2600,10 +2598,10 @@
         <v>1</v>
       </c>
       <c r="G76" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H76" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2617,10 +2615,10 @@
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H77" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2634,10 +2632,10 @@
         <v>1</v>
       </c>
       <c r="G78" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H78" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2654,38 +2652,38 @@
         <v>146</v>
       </c>
       <c r="G79" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H79" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B80" s="10" t="s">
+      <c r="B80" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C80" s="10" t="s">
+      <c r="C80" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G80" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H80" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B81" s="10" t="s">
+      <c r="B81" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C81" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G81" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H81" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.2">
@@ -2696,10 +2694,10 @@
         <v>3</v>
       </c>
       <c r="G82" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H82" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.2">
@@ -2710,10 +2708,10 @@
         <v>3</v>
       </c>
       <c r="G83" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H83" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.2">
@@ -2724,10 +2722,10 @@
         <v>3</v>
       </c>
       <c r="G84" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H84" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.2">
@@ -2738,10 +2736,10 @@
         <v>58</v>
       </c>
       <c r="G85" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H85" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.2">
@@ -2752,10 +2750,10 @@
         <v>7</v>
       </c>
       <c r="G86" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H86" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.2">
@@ -2766,58 +2764,58 @@
         <v>7</v>
       </c>
       <c r="G87" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H87" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B88" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>198</v>
+      <c r="B88" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="F88" t="s">
         <v>83</v>
       </c>
       <c r="G88" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H88" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B89" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C89" t="s">
-        <v>200</v>
+      <c r="B89" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="G89" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H89" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B90" s="8" t="s">
+      <c r="B90" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C90" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>207</v>
+      <c r="C90" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="G90" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H90" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.2">
@@ -2825,13 +2823,13 @@
         <v>62</v>
       </c>
       <c r="C91" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G91" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="H91" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.2">
@@ -2839,13 +2837,13 @@
         <v>69</v>
       </c>
       <c r="C92" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G92" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H92" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.2">
@@ -2856,17 +2854,21 @@
         <v>3</v>
       </c>
       <c r="G93" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H93" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E97" s="4"/>
+      <c r="E97" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="I15:M16"/>
     <mergeCell ref="A17:B17"/>
@@ -2875,10 +2877,6 @@
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2903,194 +2901,194 @@
       <c r="A2" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3098,19 +3096,19 @@
       <c r="A17" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3118,128 +3116,128 @@
       <c r="A18" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I21" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="I23" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="10" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="10" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3247,98 +3245,98 @@
       <c r="A27" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="10" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="10" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3346,98 +3344,98 @@
       <c r="A33" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H33" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I33" s="11" t="s">
+      <c r="I33" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H35" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I35" s="11" t="s">
+      <c r="I35" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H37" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I37" s="11" t="s">
+      <c r="I37" s="10" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="10" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
continua la modificacion de esquemas
</commit_message>
<xml_diff>
--- a/doc/schemas.xlsx
+++ b/doc/schemas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11219"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1840" windowWidth="31120" windowHeight="17440" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
+    <workbookView xWindow="3300" yWindow="1720" windowWidth="31120" windowHeight="18660" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Schemas" sheetId="1" r:id="rId1"/>
-    <sheet name="RBAC" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="RBAC" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="370">
   <si>
     <t>Collections</t>
   </si>
   <si>
-    <t>tenants</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -79,9 +77,6 @@
     <t>Cadena</t>
   </si>
   <si>
-    <t>Tenant.name</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -91,9 +86,6 @@
     <t>[String]</t>
   </si>
   <si>
-    <t>Tenant.alias[]</t>
-  </si>
-  <si>
     <t>orgUnits</t>
   </si>
   <si>
@@ -169,9 +161,6 @@
     <t>User.roles</t>
   </si>
   <si>
-    <t>Courses</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -202,9 +191,6 @@
     <t>isVerified</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
@@ -235,9 +221,6 @@
     <t>rules</t>
   </si>
   <si>
-    <t>questionaries</t>
-  </si>
-  <si>
     <t>questions</t>
   </si>
   <si>
@@ -391,9 +374,6 @@
     <t>ref 'roles'</t>
   </si>
   <si>
-    <t>ref 'tenants'</t>
-  </si>
-  <si>
     <t>org</t>
   </si>
   <si>
@@ -682,9 +662,6 @@
     <t>Para futuro uso</t>
   </si>
   <si>
-    <t>[ref 'questionaries']</t>
-  </si>
-  <si>
     <t>[ref 'questionnaries']</t>
   </si>
   <si>
@@ -790,9 +767,6 @@
     <t>[ref 'blocks']</t>
   </si>
   <si>
-    <t>course.questionaries[]</t>
-  </si>
-  <si>
     <t>course.status</t>
   </si>
   <si>
@@ -835,9 +809,6 @@
     <t>Bloques que componen el curso</t>
   </si>
   <si>
-    <t>Cuestionarios que componen el curso</t>
-  </si>
-  <si>
     <t>Estado del curso</t>
   </si>
   <si>
@@ -868,12 +839,6 @@
     <t>Titulo del bloque</t>
   </si>
   <si>
-    <t>Sección del bloque</t>
-  </si>
-  <si>
-    <t>número de bloque</t>
-  </si>
-  <si>
     <t>Contenido del bloque</t>
   </si>
   <si>
@@ -917,13 +882,268 @@
   </si>
   <si>
     <t>[{modified}]</t>
+  </si>
+  <si>
+    <t>sessions</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Usuario que inició sesión</t>
+  </si>
+  <si>
+    <t>Fecha de inicio de sesión</t>
+  </si>
+  <si>
+    <t>Sesión activa  (no sé si esta bandera deba ir)</t>
+  </si>
+  <si>
+    <t>courses</t>
+  </si>
+  <si>
+    <t>[{sessionUnit}]</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>sessionUnits</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>ref 'courses'</t>
+  </si>
+  <si>
+    <t>tracks</t>
+  </si>
+  <si>
+    <t>block.code</t>
+  </si>
+  <si>
+    <t>Código del bloque</t>
+  </si>
+  <si>
+    <t>Este bloque debe corresponder al curso que se está tomando</t>
+  </si>
+  <si>
+    <t>Usuario (alumno) que se está registrando</t>
+  </si>
+  <si>
+    <t>blockCompleted</t>
+  </si>
+  <si>
+    <t>tasks</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>versión de la tarea</t>
+  </si>
+  <si>
+    <t>palabras clave. Sirven para buscar la tarea</t>
+  </si>
+  <si>
+    <t>block.taskFormat[]</t>
+  </si>
+  <si>
+    <t>students</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>ref 'groups'</t>
+  </si>
+  <si>
+    <t>instructor</t>
+  </si>
+  <si>
+    <t>[ref 'users']</t>
+  </si>
+  <si>
+    <t>título de la tarea</t>
+  </si>
+  <si>
+    <t>descripción de la tarea</t>
+  </si>
+  <si>
+    <t>contenido de la tarea</t>
+  </si>
+  <si>
+    <t>archivos de la tarea (que deja el autor)</t>
+  </si>
+  <si>
+    <t>Nombre del grupo</t>
+  </si>
+  <si>
+    <t>Código de grupo</t>
+  </si>
+  <si>
+    <t>Curso ligado</t>
+  </si>
+  <si>
+    <t>usuario instructor (si el curso es tutoreado)</t>
+  </si>
+  <si>
+    <t>arreglo de estudiantes</t>
+  </si>
+  <si>
+    <t>beginDate</t>
+  </si>
+  <si>
+    <t>Fecha de inicio del curso/grupo</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>Fecha de fin del curso/grupo</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>session.reg[]</t>
+  </si>
+  <si>
+    <t>session.reg[].user</t>
+  </si>
+  <si>
+    <t>session.reg[].date</t>
+  </si>
+  <si>
+    <t>session.reg[].isActive</t>
+  </si>
+  <si>
+    <t>task.title</t>
+  </si>
+  <si>
+    <t>task.description</t>
+  </si>
+  <si>
+    <t>task.content</t>
+  </si>
+  <si>
+    <t>task.file[]</t>
+  </si>
+  <si>
+    <t>task.version</t>
+  </si>
+  <si>
+    <t>task.keywords[]</t>
+  </si>
+  <si>
+    <t>task.isVisible</t>
+  </si>
+  <si>
+    <t>task.own</t>
+  </si>
+  <si>
+    <t>task.mod</t>
+  </si>
+  <si>
+    <t>task.perm</t>
+  </si>
+  <si>
+    <t>track.user</t>
+  </si>
+  <si>
+    <t>track.blockCompleted</t>
+  </si>
+  <si>
+    <t>track.course</t>
+  </si>
+  <si>
+    <t>track.group</t>
+  </si>
+  <si>
+    <t>ref 'orgs'</t>
+  </si>
+  <si>
+    <t>[ref 'orgUnit']</t>
+  </si>
+  <si>
+    <t>Contenidos del curso</t>
+  </si>
+  <si>
+    <t>Sección</t>
+  </si>
+  <si>
+    <t>Bloque</t>
+  </si>
+  <si>
+    <t>Introducción a las matemáticas</t>
+  </si>
+  <si>
+    <t>Origen de las matemáticas</t>
+  </si>
+  <si>
+    <t>bloque</t>
+  </si>
+  <si>
+    <t>Historia</t>
+  </si>
+  <si>
+    <t>Temario</t>
+  </si>
+  <si>
+    <t>Syllabus</t>
+  </si>
+  <si>
+    <t>[ref 'block']</t>
+  </si>
+  <si>
+    <t>Org.name</t>
+  </si>
+  <si>
+    <t>Org.alias[]</t>
+  </si>
+  <si>
+    <t>Número de bloque dentro de la sección. Bloque 0 es la sección</t>
+  </si>
+  <si>
+    <t>Sección a la que pertecene el bloque (bloque 0 es el que corresponde a la sección en sí)</t>
+  </si>
+  <si>
+    <t>[ref 'tasks']</t>
+  </si>
+  <si>
+    <t>Tareas del bloque</t>
+  </si>
+  <si>
+    <t>["text","textVideo","video","task","questionnarie"]</t>
+  </si>
+  <si>
+    <t>block.type</t>
+  </si>
+  <si>
+    <t>Tipo de código</t>
+  </si>
+  <si>
+    <t>curso sobre el que se hace tracking</t>
+  </si>
+  <si>
+    <t>grupo sobre el que se hace tracking</t>
+  </si>
+  <si>
+    <t>weights</t>
+  </si>
+  <si>
+    <t>[ref 'orgs']</t>
+  </si>
+  <si>
+    <t>ref 'course'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -995,6 +1215,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1046,7 +1272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1076,6 +1302,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1396,11 +1626,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB6E249-7676-0040-9A74-86494BA4AA54}">
-  <dimension ref="A1:M97"/>
+  <dimension ref="A1:M140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B88" sqref="B88:C90"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1420,251 +1650,240 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>356</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="17"/>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>357</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
+      <c r="A7" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="19"/>
       <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>123</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" t="s">
+        <v>344</v>
+      </c>
+      <c r="G12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H12" t="s">
         <v>121</v>
       </c>
-      <c r="G11" t="s">
-        <v>127</v>
-      </c>
-      <c r="H11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
+      <c r="A13" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="19"/>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="B14" s="17"/>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>179</v>
-      </c>
+      <c r="A15" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="19"/>
       <c r="C15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G15" t="s">
-        <v>200</v>
-      </c>
-      <c r="H15" t="s">
-        <v>294</v>
-      </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
+        <v>134</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C16" t="s">
-        <v>293</v>
+        <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H16" t="s">
-        <v>295</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
+        <v>282</v>
+      </c>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="B17" s="17"/>
+      <c r="B17" t="s">
+        <v>173</v>
+      </c>
       <c r="C17" t="s">
-        <v>141</v>
-      </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
+        <v>281</v>
+      </c>
+      <c r="F17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" t="s">
+        <v>194</v>
+      </c>
+      <c r="H17" t="s">
+        <v>283</v>
+      </c>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>113</v>
-      </c>
+      <c r="A18" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="19"/>
       <c r="C18" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" t="s">
-        <v>183</v>
-      </c>
-      <c r="H18" t="s">
-        <v>186</v>
+        <v>134</v>
       </c>
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
@@ -1674,16 +1893,16 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H19" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="I19" s="16"/>
       <c r="J19" s="16"/>
@@ -1693,16 +1912,16 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H20" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
@@ -1711,1172 +1930,1630 @@
       <c r="M20" s="16"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="17"/>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
       <c r="C21" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>178</v>
+      </c>
+      <c r="H21" t="s">
+        <v>181</v>
+      </c>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
+      <c r="A22" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="19"/>
       <c r="C22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
       </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H23" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>122</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>148</v>
+        <v>35</v>
       </c>
       <c r="G25" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H25" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="H26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="G27" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="H27" t="s">
-        <v>150</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B28" s="9" t="s">
-        <v>56</v>
+      <c r="B28" t="s">
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" t="b">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="G28" t="s">
-        <v>149</v>
+        <v>43</v>
       </c>
       <c r="H28" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>142</v>
+      </c>
+      <c r="H29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" t="b">
         <v>0</v>
       </c>
-      <c r="G29" t="s">
-        <v>152</v>
-      </c>
-      <c r="H29" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B30" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C30" t="s">
-        <v>296</v>
-      </c>
       <c r="G30" t="s">
-        <v>198</v>
+        <v>145</v>
       </c>
       <c r="H30" t="s">
-        <v>199</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B31" s="17"/>
+      <c r="B31" s="4" t="s">
+        <v>202</v>
+      </c>
       <c r="C31" t="s">
-        <v>141</v>
+        <v>284</v>
+      </c>
+      <c r="G31" t="s">
+        <v>191</v>
+      </c>
+      <c r="H31" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>132</v>
-      </c>
+      <c r="A32" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="19"/>
       <c r="C32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>154</v>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
-      </c>
-      <c r="G32" t="s">
-        <v>189</v>
-      </c>
-      <c r="H32" t="s">
-        <v>157</v>
-      </c>
-      <c r="J32" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="H33" t="s">
-        <v>158</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>181</v>
+        <v>150</v>
+      </c>
+      <c r="J33" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="H34" t="s">
-        <v>159</v>
-      </c>
-      <c r="J34" s="4"/>
+        <v>151</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="K34" s="4" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B35" s="17"/>
+      <c r="B35" t="s">
+        <v>127</v>
+      </c>
       <c r="C35" t="s">
-        <v>141</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>87</v>
+        <v>41</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>184</v>
+      </c>
+      <c r="H35" t="s">
+        <v>152</v>
+      </c>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>63</v>
-      </c>
+      <c r="A36" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="19"/>
       <c r="C36" t="s">
-        <v>139</v>
-      </c>
-      <c r="E36" t="s">
-        <v>154</v>
-      </c>
-      <c r="G36" t="s">
-        <v>166</v>
-      </c>
-      <c r="H36" t="s">
-        <v>160</v>
-      </c>
-      <c r="J36" s="6"/>
+        <v>134</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="K36" s="6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E37" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G37" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="H37" t="s">
-        <v>161</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K37" s="7" t="s">
-        <v>84</v>
+        <v>153</v>
+      </c>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>140</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E38" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" t="s">
+        <v>160</v>
+      </c>
+      <c r="H38" t="s">
         <v>154</v>
       </c>
-      <c r="G38" t="s">
-        <v>168</v>
-      </c>
-      <c r="H38" t="s">
-        <v>163</v>
-      </c>
-      <c r="J38" s="7"/>
+      <c r="J38" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="K38" s="7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E39" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G39" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="H39" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="J39" s="7"/>
       <c r="K39" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="17"/>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
       <c r="C40" t="s">
-        <v>23</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="K40" s="8"/>
+        <v>132</v>
+      </c>
+      <c r="E40" t="s">
+        <v>147</v>
+      </c>
+      <c r="G40" t="s">
+        <v>162</v>
+      </c>
+      <c r="H40" t="s">
+        <v>155</v>
+      </c>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>71</v>
-      </c>
+      <c r="A41" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="19"/>
       <c r="C41" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" t="b">
-        <v>1</v>
-      </c>
-      <c r="G41" t="s">
-        <v>165</v>
-      </c>
-      <c r="H41" t="s">
-        <v>172</v>
-      </c>
-      <c r="J41" s="9" t="s">
-        <v>90</v>
+        <v>20</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="K41" s="8"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="H42" t="s">
-        <v>173</v>
-      </c>
-      <c r="J42" s="9"/>
+        <v>165</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="K42" s="8"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="D43" t="b">
+        <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="H43" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="J43" s="9"/>
       <c r="K43" s="8"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G44" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H44" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="8"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>44</v>
+      <c r="B45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
       </c>
       <c r="G45" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="H45" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="8"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F46" t="s">
-        <v>83</v>
+      <c r="B46" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="G46" t="s">
-        <v>228</v>
+        <v>163</v>
       </c>
       <c r="H46" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="8"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B47" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>296</v>
+      <c r="B47" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F47" t="s">
+        <v>77</v>
       </c>
       <c r="G47" t="s">
-        <v>229</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="H47" t="s">
+        <v>196</v>
+      </c>
+      <c r="J47" s="9"/>
+      <c r="K47" s="8"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B48" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="B48" s="4" t="s">
         <v>202</v>
       </c>
+      <c r="C48" s="4" t="s">
+        <v>284</v>
+      </c>
       <c r="G48" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B49" s="17"/>
-      <c r="C49" t="s">
-        <v>13</v>
+      <c r="B49" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F49" t="s">
+        <v>195</v>
+      </c>
+      <c r="G49" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
-        <v>4</v>
-      </c>
+      <c r="A50" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" s="19"/>
       <c r="C50" t="s">
-        <v>3</v>
-      </c>
-      <c r="G50" t="s">
-        <v>192</v>
-      </c>
-      <c r="H50" t="s">
-        <v>232</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="G51" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="H51" t="s">
-        <v>271</v>
+        <v>224</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>3</v>
+      <c r="B52" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" t="s">
+        <v>66</v>
       </c>
       <c r="G52" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="H52" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B53" s="9" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G53" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="H53" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B54" s="9" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G54" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H54" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F55" t="s">
-        <v>83</v>
+      <c r="B55" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="G55" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="H55" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>296</v>
+      <c r="B56" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F56" t="s">
+        <v>77</v>
       </c>
       <c r="G56" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="H56" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="B57" s="4" t="s">
         <v>202</v>
       </c>
+      <c r="C57" s="4" t="s">
+        <v>284</v>
+      </c>
       <c r="G57" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="H57" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" s="1"/>
-      <c r="C58" t="s">
-        <v>13</v>
+      <c r="B58" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F58" t="s">
+        <v>195</v>
+      </c>
+      <c r="G58" t="s">
+        <v>200</v>
+      </c>
+      <c r="H58" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>49</v>
-      </c>
-      <c r="C59" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" t="b">
-        <v>1</v>
-      </c>
-      <c r="G59" t="s">
-        <v>210</v>
-      </c>
-      <c r="H59" t="s">
-        <v>279</v>
+      <c r="A59" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="B59" s="19"/>
+      <c r="C59" s="18" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60" t="b">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G60" t="s">
-        <v>211</v>
+        <v>330</v>
       </c>
       <c r="H60" t="s">
-        <v>280</v>
+        <v>312</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C61" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" t="b">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G61" t="s">
-        <v>212</v>
+        <v>331</v>
       </c>
       <c r="H61" t="s">
-        <v>281</v>
+        <v>313</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" t="b">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G62" t="s">
-        <v>213</v>
+        <v>332</v>
       </c>
       <c r="H62" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>66</v>
+        <v>303</v>
       </c>
       <c r="C63" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63" t="s">
+        <v>333</v>
+      </c>
+      <c r="H63" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B64" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64" t="s">
+        <v>334</v>
+      </c>
+      <c r="H64" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B65" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" t="s">
+        <v>335</v>
+      </c>
+      <c r="H65" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B66" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G66" t="s">
+        <v>336</v>
+      </c>
+      <c r="H66" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B67" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G67" t="s">
+        <v>337</v>
+      </c>
+      <c r="H67" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B68" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="G68" t="s">
+        <v>338</v>
+      </c>
+      <c r="H68" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B69" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="G69" t="s">
+        <v>339</v>
+      </c>
+      <c r="H69" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>44</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" t="b">
+        <v>1</v>
+      </c>
+      <c r="G71" t="s">
+        <v>297</v>
+      </c>
+      <c r="H71" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
         <v>3</v>
       </c>
-      <c r="G63" t="s">
-        <v>214</v>
-      </c>
-      <c r="H63" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>67</v>
-      </c>
-      <c r="C64" t="s">
-        <v>20</v>
-      </c>
-      <c r="G64" t="s">
-        <v>215</v>
-      </c>
-      <c r="H64" s="15" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
-        <v>68</v>
-      </c>
-      <c r="C65" t="s">
-        <v>20</v>
-      </c>
-      <c r="G65" t="s">
-        <v>216</v>
-      </c>
-      <c r="H65" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
-        <v>164</v>
-      </c>
-      <c r="C66" t="s">
-        <v>219</v>
-      </c>
-      <c r="G66" t="s">
-        <v>220</v>
-      </c>
-      <c r="H66" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
-        <v>76</v>
-      </c>
-      <c r="C67" t="s">
-        <v>3</v>
-      </c>
-      <c r="G67" t="s">
-        <v>221</v>
-      </c>
-      <c r="H67" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B68" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G68" t="s">
-        <v>222</v>
-      </c>
-      <c r="H68" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G69" t="s">
-        <v>223</v>
-      </c>
-      <c r="H69" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B70" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G70" t="s">
-        <v>224</v>
-      </c>
-      <c r="H70" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B71" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F71" t="s">
-        <v>83</v>
-      </c>
-      <c r="G71" t="s">
-        <v>225</v>
-      </c>
-      <c r="H71" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B72" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>296</v>
+      <c r="C72" t="s">
+        <v>362</v>
       </c>
       <c r="G72" t="s">
-        <v>226</v>
+        <v>363</v>
       </c>
       <c r="H72" t="s">
-        <v>290</v>
+        <v>364</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F73" t="s">
-        <v>202</v>
+      <c r="B73" t="s">
+        <v>45</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" t="b">
+        <v>1</v>
       </c>
       <c r="G73" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="H73" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B74" s="17"/>
+      <c r="B74" t="s">
+        <v>60</v>
+      </c>
       <c r="C74" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="D74" t="b">
+        <v>1</v>
+      </c>
+      <c r="G74" t="s">
+        <v>204</v>
+      </c>
+      <c r="H74" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C75" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D75" t="b">
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="H75" t="s">
-        <v>256</v>
+        <v>358</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="C76" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D76" t="b">
         <v>1</v>
       </c>
       <c r="G76" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="H76" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="C77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D77" t="b">
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="H77" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="C78" t="s">
-        <v>3</v>
-      </c>
-      <c r="D78" t="b">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G78" t="s">
-        <v>239</v>
-      </c>
-      <c r="H78" t="s">
-        <v>233</v>
+        <v>208</v>
+      </c>
+      <c r="H78" s="15" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>145</v>
+        <v>63</v>
       </c>
       <c r="C79" t="s">
-        <v>20</v>
-      </c>
-      <c r="D79" t="b">
+        <v>18</v>
+      </c>
+      <c r="G79" t="s">
+        <v>209</v>
+      </c>
+      <c r="H79" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" t="s">
+        <v>211</v>
+      </c>
+      <c r="G80" t="s">
+        <v>212</v>
+      </c>
+      <c r="H80" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>302</v>
+      </c>
+      <c r="C81" t="s">
+        <v>360</v>
+      </c>
+      <c r="G81" t="s">
+        <v>306</v>
+      </c>
+      <c r="H81" s="15" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>70</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+      <c r="G82" t="s">
+        <v>213</v>
+      </c>
+      <c r="H82" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B83" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G83" t="s">
+        <v>214</v>
+      </c>
+      <c r="H83" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B84" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G84" t="s">
+        <v>215</v>
+      </c>
+      <c r="H84" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B85" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G85" t="s">
+        <v>216</v>
+      </c>
+      <c r="H85" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B86" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F86" t="s">
+        <v>77</v>
+      </c>
+      <c r="G86" t="s">
+        <v>217</v>
+      </c>
+      <c r="H86" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B87" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="G87" t="s">
+        <v>218</v>
+      </c>
+      <c r="H87" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B88" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F88" t="s">
+        <v>195</v>
+      </c>
+      <c r="G88" t="s">
+        <v>219</v>
+      </c>
+      <c r="H88" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="B90" s="17"/>
+      <c r="C90" s="7"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>294</v>
+      </c>
+      <c r="C91" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B101" s="19"/>
+      <c r="C101" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>44</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" t="b">
         <v>1</v>
       </c>
-      <c r="E79" t="s">
-        <v>146</v>
-      </c>
-      <c r="G79" t="s">
+      <c r="G102" t="s">
+        <v>228</v>
+      </c>
+      <c r="H102" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>45</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+      <c r="G103" t="s">
+        <v>229</v>
+      </c>
+      <c r="H103" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>2</v>
+      </c>
+      <c r="D104" t="b">
+        <v>1</v>
+      </c>
+      <c r="G104" t="s">
+        <v>230</v>
+      </c>
+      <c r="H104" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105" t="b">
+        <v>1</v>
+      </c>
+      <c r="G105" t="s">
+        <v>231</v>
+      </c>
+      <c r="H105" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>138</v>
+      </c>
+      <c r="C106" t="s">
+        <v>18</v>
+      </c>
+      <c r="D106" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" t="s">
+        <v>139</v>
+      </c>
+      <c r="G106" t="s">
+        <v>232</v>
+      </c>
+      <c r="H106" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B107" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G107" t="s">
+        <v>233</v>
+      </c>
+      <c r="H107" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B108" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G108" t="s">
+        <v>234</v>
+      </c>
+      <c r="H108" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>47</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+      <c r="G109" t="s">
+        <v>235</v>
+      </c>
+      <c r="H109" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>54</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+      <c r="G110" t="s">
+        <v>236</v>
+      </c>
+      <c r="H110" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>48</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2</v>
+      </c>
+      <c r="G111" t="s">
+        <v>237</v>
+      </c>
+      <c r="H111" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>49</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2</v>
+      </c>
+      <c r="G112" t="s">
+        <v>238</v>
+      </c>
+      <c r="H112" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>50</v>
+      </c>
+      <c r="C113" t="s">
+        <v>6</v>
+      </c>
+      <c r="G113" t="s">
+        <v>239</v>
+      </c>
+      <c r="H113" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>51</v>
+      </c>
+      <c r="C114" t="s">
+        <v>6</v>
+      </c>
+      <c r="G114" t="s">
         <v>240</v>
       </c>
-      <c r="H79" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B80" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C80" s="9" t="s">
+      <c r="H114" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B115" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F115" t="s">
+        <v>77</v>
+      </c>
+      <c r="G115" t="s">
+        <v>241</v>
+      </c>
+      <c r="H115" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B116" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="G116" t="s">
+        <v>243</v>
+      </c>
+      <c r="H116" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B117" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G117" t="s">
+        <v>242</v>
+      </c>
+      <c r="H117" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>57</v>
+      </c>
+      <c r="C118" t="s">
+        <v>245</v>
+      </c>
+      <c r="G118" t="s">
+        <v>244</v>
+      </c>
+      <c r="H118" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
+        <v>70</v>
+      </c>
+      <c r="C119" t="s">
+        <v>2</v>
+      </c>
+      <c r="G119" t="s">
+        <v>246</v>
+      </c>
+      <c r="H119" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B120" s="19"/>
+      <c r="C120" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
+        <v>107</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2</v>
+      </c>
+      <c r="G121" t="s">
+        <v>327</v>
+      </c>
+      <c r="H121" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B122" t="s">
+        <v>286</v>
+      </c>
+      <c r="C122" t="s">
+        <v>281</v>
+      </c>
+      <c r="G122" t="s">
+        <v>328</v>
+      </c>
+      <c r="H122" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B123" t="s">
+        <v>52</v>
+      </c>
+      <c r="C123" t="s">
+        <v>41</v>
+      </c>
+      <c r="G123" t="s">
+        <v>329</v>
+      </c>
+      <c r="H123" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="B124" s="19"/>
+      <c r="C124" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B125" t="s">
+        <v>325</v>
+      </c>
+      <c r="C125" t="s">
+        <v>291</v>
+      </c>
+      <c r="E125" s="3"/>
+      <c r="G125" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B126" s="19"/>
+      <c r="C126" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B127" t="s">
+        <v>107</v>
+      </c>
+      <c r="C127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G127" t="s">
+        <v>340</v>
+      </c>
+      <c r="H127" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B128" t="s">
+        <v>301</v>
+      </c>
+      <c r="C128" t="s">
+        <v>355</v>
+      </c>
+      <c r="G128" t="s">
+        <v>341</v>
+      </c>
+      <c r="H128" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B129" t="s">
+        <v>294</v>
+      </c>
+      <c r="C129" t="s">
+        <v>295</v>
+      </c>
+      <c r="G129" t="s">
+        <v>342</v>
+      </c>
+      <c r="H129" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B130" t="s">
+        <v>308</v>
+      </c>
+      <c r="C130" t="s">
+        <v>309</v>
+      </c>
+      <c r="G130" t="s">
+        <v>343</v>
+      </c>
+      <c r="H130" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B131" s="19"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B132" t="s">
         <v>44</v>
       </c>
-      <c r="G80" t="s">
-        <v>241</v>
-      </c>
-      <c r="H80" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B81" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G81" t="s">
-        <v>242</v>
-      </c>
-      <c r="H81" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B82" t="s">
-        <v>51</v>
-      </c>
-      <c r="C82" t="s">
-        <v>3</v>
-      </c>
-      <c r="G82" t="s">
-        <v>243</v>
-      </c>
-      <c r="H82" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B83" t="s">
-        <v>59</v>
-      </c>
-      <c r="C83" t="s">
-        <v>3</v>
-      </c>
-      <c r="G83" t="s">
-        <v>244</v>
-      </c>
-      <c r="H83" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
-        <v>52</v>
-      </c>
-      <c r="C84" t="s">
-        <v>3</v>
-      </c>
-      <c r="G84" t="s">
-        <v>245</v>
-      </c>
-      <c r="H84" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B85" t="s">
-        <v>53</v>
-      </c>
-      <c r="C85" t="s">
-        <v>58</v>
-      </c>
-      <c r="G85" t="s">
-        <v>246</v>
-      </c>
-      <c r="H85" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B86" t="s">
-        <v>54</v>
-      </c>
-      <c r="C86" t="s">
-        <v>7</v>
-      </c>
-      <c r="G86" t="s">
-        <v>247</v>
-      </c>
-      <c r="H86" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B87" t="s">
-        <v>55</v>
-      </c>
-      <c r="C87" t="s">
-        <v>7</v>
-      </c>
-      <c r="G87" t="s">
-        <v>248</v>
-      </c>
-      <c r="H87" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B88" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F88" t="s">
-        <v>83</v>
-      </c>
-      <c r="G88" t="s">
-        <v>249</v>
-      </c>
-      <c r="H88" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B89" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="G89" t="s">
-        <v>251</v>
-      </c>
-      <c r="H89" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B90" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G90" t="s">
-        <v>250</v>
-      </c>
-      <c r="H90" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B91" t="s">
-        <v>62</v>
-      </c>
-      <c r="C91" t="s">
-        <v>253</v>
-      </c>
-      <c r="G91" t="s">
-        <v>252</v>
-      </c>
-      <c r="H91" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
-        <v>69</v>
-      </c>
-      <c r="C92" t="s">
-        <v>218</v>
-      </c>
-      <c r="G92" t="s">
-        <v>254</v>
-      </c>
-      <c r="H92" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
-        <v>76</v>
-      </c>
-      <c r="C93" t="s">
-        <v>3</v>
-      </c>
-      <c r="G93" t="s">
-        <v>255</v>
-      </c>
-      <c r="H93" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E97" s="3"/>
+      <c r="C132" t="s">
+        <v>2</v>
+      </c>
+      <c r="H132" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B133" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s">
+        <v>2</v>
+      </c>
+      <c r="H133" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
+        <v>294</v>
+      </c>
+      <c r="C134" t="s">
+        <v>295</v>
+      </c>
+      <c r="H134" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B135" t="s">
+        <v>310</v>
+      </c>
+      <c r="C135" t="s">
+        <v>73</v>
+      </c>
+      <c r="H135" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B136" t="s">
+        <v>307</v>
+      </c>
+      <c r="C136" t="s">
+        <v>311</v>
+      </c>
+      <c r="H136" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B137" t="s">
+        <v>321</v>
+      </c>
+      <c r="C137" t="s">
+        <v>281</v>
+      </c>
+      <c r="H137" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B138" t="s">
+        <v>323</v>
+      </c>
+      <c r="C138" t="s">
+        <v>281</v>
+      </c>
+      <c r="H138" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B139" t="s">
+        <v>115</v>
+      </c>
+      <c r="C139" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B140" t="s">
+        <v>67</v>
+      </c>
+      <c r="C140" t="s">
+        <v>345</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="17">
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="I15:M16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="I16:M17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A59:B59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2884,6 +3561,66 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F12A2F9-1AE6-3C42-AA72-B6D7679A6D69}">
+  <dimension ref="B2:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="282" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="3.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>348</v>
+      </c>
+      <c r="D4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5">
+        <v>1.2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AEAD6A-92F9-7A48-A434-AB75EEB17EE7}">
   <dimension ref="A2:I38"/>
   <sheetViews>
@@ -2899,162 +3636,162 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>98</v>
-      </c>
       <c r="C9" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -3074,62 +3811,62 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -3144,299 +3881,299 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E21" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" s="10" t="s">
         <v>113</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E22" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C23" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E23" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>120</v>
-      </c>
       <c r="G23" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E24" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C25" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E26" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E27" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I27" s="10" t="s">
         <v>113</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E28" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C29" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E29" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>120</v>
-      </c>
       <c r="G29" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E30" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C31" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E32" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E33" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I33" s="10" t="s">
         <v>113</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E34" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C35" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E35" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F35" s="10" t="s">
-        <v>120</v>
-      </c>
       <c r="G35" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E36" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C37" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E38" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3444,7 +4181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12457892-A860-024C-BFC8-6E106FE379AF}">
   <dimension ref="A3:E14"/>
   <sheetViews>
@@ -3456,83 +4193,83 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando api para modificar propiedades del usuario
</commit_message>
<xml_diff>
--- a/doc/schemas.xlsx
+++ b/doc/schemas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11219"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1420" windowWidth="31120" windowHeight="18660" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
+    <workbookView xWindow="14720" yWindow="2180" windowWidth="31120" windowHeight="18660" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Schemas" sheetId="1" r:id="rId1"/>
@@ -1392,8 +1392,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1794,15 +1794,6 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1821,7 +1812,7 @@
     <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1830,11 +1821,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2183,8 +2183,8 @@
   <dimension ref="A1:M162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2229,10 +2229,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="39"/>
+      <c r="B3" s="51"/>
       <c r="C3" t="s">
         <v>12</v>
       </c>
@@ -2334,10 +2334,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="39"/>
+      <c r="B10" s="51"/>
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -2464,10 +2464,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="39"/>
+      <c r="B19" s="51"/>
       <c r="C19" t="s">
         <v>12</v>
       </c>
@@ -2481,10 +2481,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="39"/>
+      <c r="B21" s="51"/>
       <c r="C21" t="s">
         <v>111</v>
       </c>
@@ -2505,11 +2505,11 @@
       <c r="H22" t="s">
         <v>253</v>
       </c>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
@@ -2527,17 +2527,17 @@
       <c r="H23" t="s">
         <v>254</v>
       </c>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="39"/>
+      <c r="B24" s="51"/>
       <c r="C24" t="s">
         <v>111</v>
       </c>
@@ -2605,10 +2605,10 @@
       <c r="M27" s="15"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="39"/>
+      <c r="B28" s="51"/>
       <c r="C28" t="s">
         <v>111</v>
       </c>
@@ -2729,10 +2729,10 @@
       <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="39"/>
+      <c r="B34" s="51"/>
       <c r="C34" t="s">
         <v>12</v>
       </c>
@@ -2896,10 +2896,10 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="39"/>
+      <c r="B45" s="51"/>
       <c r="C45" t="s">
         <v>111</v>
       </c>
@@ -2980,10 +2980,10 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="39"/>
+      <c r="B49" s="51"/>
       <c r="C49" t="s">
         <v>111</v>
       </c>
@@ -3057,10 +3057,10 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="39" t="s">
+      <c r="A54" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="39"/>
+      <c r="B54" s="51"/>
       <c r="C54" t="s">
         <v>19</v>
       </c>
@@ -3184,10 +3184,10 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="39" t="s">
+      <c r="A63" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="B63" s="39"/>
+      <c r="B63" s="51"/>
       <c r="C63" t="s">
         <v>12</v>
       </c>
@@ -3202,7 +3202,7 @@
       <c r="D64" t="b">
         <v>1</v>
       </c>
-      <c r="F64" s="53" t="s">
+      <c r="F64" s="49" t="s">
         <v>438</v>
       </c>
       <c r="G64" t="s">
@@ -3337,10 +3337,10 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="39" t="s">
+      <c r="A73" s="51" t="s">
         <v>273</v>
       </c>
-      <c r="B73" s="39"/>
+      <c r="B73" s="51"/>
       <c r="C73" s="16" t="s">
         <v>12</v>
       </c>
@@ -3871,10 +3871,10 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="39" t="s">
+      <c r="A110" s="51" t="s">
         <v>261</v>
       </c>
-      <c r="B110" s="39"/>
+      <c r="B110" s="51"/>
       <c r="C110" t="s">
         <v>12</v>
       </c>
@@ -4159,10 +4159,10 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="39" t="s">
+      <c r="A129" s="51" t="s">
         <v>264</v>
       </c>
-      <c r="B129" s="39"/>
+      <c r="B129" s="51"/>
       <c r="C129" t="s">
         <v>111</v>
       </c>
@@ -4210,10 +4210,10 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A133" s="39" t="s">
+      <c r="A133" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="B133" s="39"/>
+      <c r="B133" s="51"/>
       <c r="C133" t="s">
         <v>12</v>
       </c>
@@ -4231,10 +4231,10 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="39" t="s">
+      <c r="A135" s="51" t="s">
         <v>267</v>
       </c>
-      <c r="B135" s="39"/>
+      <c r="B135" s="51"/>
       <c r="C135" t="s">
         <v>12</v>
       </c>
@@ -4299,10 +4299,10 @@
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="39" t="s">
+      <c r="A140" s="51" t="s">
         <v>383</v>
       </c>
-      <c r="B140" s="39"/>
+      <c r="B140" s="51"/>
       <c r="C140" t="s">
         <v>19</v>
       </c>
@@ -4350,10 +4350,10 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="39" t="s">
+      <c r="A144" s="51" t="s">
         <v>380</v>
       </c>
-      <c r="B144" s="39"/>
+      <c r="B144" s="51"/>
       <c r="C144" t="s">
         <v>111</v>
       </c>
@@ -4390,10 +4390,10 @@
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A147" s="39" t="s">
+      <c r="A147" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="B147" s="39"/>
+      <c r="B147" s="51"/>
       <c r="C147" t="s">
         <v>111</v>
       </c>
@@ -4446,10 +4446,10 @@
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A152" s="39" t="s">
+      <c r="A152" s="51" t="s">
         <v>263</v>
       </c>
-      <c r="B152" s="39"/>
+      <c r="B152" s="51"/>
       <c r="C152" t="s">
         <v>12</v>
       </c>
@@ -4565,13 +4565,13 @@
       <c r="H160" t="s">
         <v>376</v>
       </c>
-      <c r="I160" s="51" t="s">
+      <c r="I160" s="50" t="s">
         <v>379</v>
       </c>
-      <c r="J160" s="51"/>
-      <c r="K160" s="51"/>
-      <c r="L160" s="51"/>
-      <c r="M160" s="51"/>
+      <c r="J160" s="50"/>
+      <c r="K160" s="50"/>
+      <c r="L160" s="50"/>
+      <c r="M160" s="50"/>
     </row>
     <row r="161" spans="2:13" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
@@ -4586,13 +4586,13 @@
       <c r="H161" t="s">
         <v>377</v>
       </c>
-      <c r="I161" s="51" t="s">
+      <c r="I161" s="50" t="s">
         <v>378</v>
       </c>
-      <c r="J161" s="51"/>
-      <c r="K161" s="51"/>
-      <c r="L161" s="51"/>
-      <c r="M161" s="51"/>
+      <c r="J161" s="50"/>
+      <c r="K161" s="50"/>
+      <c r="L161" s="50"/>
+      <c r="M161" s="50"/>
     </row>
     <row r="162" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
@@ -4608,16 +4608,11 @@
   </sheetData>
   <autoFilter ref="A2:M161" xr:uid="{A98571A1-046A-F843-AA6D-99F644BB2C36}"/>
   <mergeCells count="23">
-    <mergeCell ref="I161:M161"/>
-    <mergeCell ref="I160:M160"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="I22:M23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A110:B110"/>
@@ -4626,11 +4621,16 @@
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="I161:M161"/>
+    <mergeCell ref="I160:M160"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A147:B147"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4694,7 +4694,7 @@
       <c r="B3" t="s">
         <v>315</v>
       </c>
-      <c r="D3" s="52">
+      <c r="D3" s="48">
         <v>1</v>
       </c>
       <c r="E3" t="s">
@@ -5355,7 +5355,7 @@
       <c r="R7" s="31">
         <v>4</v>
       </c>
-      <c r="S7" s="41" t="s">
+      <c r="S7" s="53" t="s">
         <v>340</v>
       </c>
     </row>
@@ -5414,7 +5414,7 @@
       <c r="R8" s="32">
         <v>0</v>
       </c>
-      <c r="S8" s="41"/>
+      <c r="S8" s="53"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -5471,7 +5471,7 @@
       <c r="R9" s="19">
         <v>0</v>
       </c>
-      <c r="S9" s="41"/>
+      <c r="S9" s="53"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
@@ -5528,7 +5528,7 @@
       <c r="R10" s="34">
         <v>0</v>
       </c>
-      <c r="S10" s="41"/>
+      <c r="S10" s="53"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -5563,7 +5563,7 @@
         <f>R9*R10*R15</f>
         <v>0</v>
       </c>
-      <c r="S11" s="41"/>
+      <c r="S11" s="53"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -5620,7 +5620,7 @@
       <c r="R12" s="19">
         <v>1</v>
       </c>
-      <c r="S12" s="41"/>
+      <c r="S12" s="53"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
@@ -5677,7 +5677,7 @@
       <c r="R13" s="34">
         <v>1</v>
       </c>
-      <c r="S13" s="41"/>
+      <c r="S13" s="53"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -5687,7 +5687,7 @@
         <f>(B12*B13*B15)</f>
         <v>1</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C14" s="45">
         <f>(C12*C13*C15)+(D12*D13*D15)+(E12*E13*E15)+(F12*F13*F15)+(G12*G13*G15)</f>
         <v>0.745</v>
       </c>
@@ -5712,64 +5712,64 @@
         <f>R12*R13*R15</f>
         <v>0</v>
       </c>
-      <c r="S14" s="41"/>
+      <c r="S14" s="53"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>342</v>
       </c>
-      <c r="B15" s="42">
-        <v>1</v>
-      </c>
-      <c r="C15" s="43">
-        <v>1</v>
-      </c>
-      <c r="D15" s="44">
-        <v>1</v>
-      </c>
-      <c r="E15" s="44">
-        <v>1</v>
-      </c>
-      <c r="F15" s="44">
-        <v>1</v>
-      </c>
-      <c r="G15" s="45">
-        <v>1</v>
-      </c>
-      <c r="H15" s="43">
+      <c r="B15" s="39">
+        <v>1</v>
+      </c>
+      <c r="C15" s="40">
+        <v>1</v>
+      </c>
+      <c r="D15" s="41">
+        <v>1</v>
+      </c>
+      <c r="E15" s="41">
+        <v>1</v>
+      </c>
+      <c r="F15" s="41">
+        <v>1</v>
+      </c>
+      <c r="G15" s="42">
+        <v>1</v>
+      </c>
+      <c r="H15" s="40">
         <v>0</v>
       </c>
-      <c r="I15" s="44">
+      <c r="I15" s="41">
         <v>0</v>
       </c>
-      <c r="J15" s="44">
+      <c r="J15" s="41">
         <v>0</v>
       </c>
-      <c r="K15" s="44">
+      <c r="K15" s="41">
         <v>0</v>
       </c>
-      <c r="L15" s="45">
+      <c r="L15" s="42">
         <v>0</v>
       </c>
-      <c r="M15" s="43">
+      <c r="M15" s="40">
         <v>0</v>
       </c>
-      <c r="N15" s="44">
+      <c r="N15" s="41">
         <v>0</v>
       </c>
-      <c r="O15" s="44">
+      <c r="O15" s="41">
         <v>0</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="41">
         <v>0</v>
       </c>
-      <c r="Q15" s="45">
+      <c r="Q15" s="42">
         <v>0</v>
       </c>
-      <c r="R15" s="46">
+      <c r="R15" s="43">
         <v>0</v>
       </c>
-      <c r="S15" s="47">
+      <c r="S15" s="44">
         <f>AVERAGE(B15:R15)</f>
         <v>0.35294117647058826</v>
       </c>
@@ -5795,7 +5795,7 @@
         <f>R11+R14</f>
         <v>0</v>
       </c>
-      <c r="S16" s="49">
+      <c r="S16" s="46">
         <f>(B16*B17)+(C16*C17)+(H16*H17)+(M16*M17)+(R16*R17)</f>
         <v>0.21812500000000001</v>
       </c>
@@ -5819,7 +5819,7 @@
       <c r="S17" s="37"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="47" t="s">
         <v>352</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregando inicializador de la base de datos
</commit_message>
<xml_diff>
--- a/doc/schemas.xlsx
+++ b/doc/schemas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14720" yWindow="2180" windowWidth="31120" windowHeight="18660" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
+    <workbookView xWindow="1080" yWindow="1560" windowWidth="31120" windowHeight="18660" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Schemas" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="453">
   <si>
     <t>Collections</t>
   </si>
@@ -1384,6 +1384,12 @@
   </si>
   <si>
     <t>[{dates}]</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>Para controlar las fechas por bloque y sección</t>
   </si>
 </sst>
 </file>
@@ -1823,14 +1829,14 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2183,8 +2189,8 @@
   <dimension ref="A1:M162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="2" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E156" sqref="E156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2229,10 +2235,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="51"/>
+      <c r="B3" s="50"/>
       <c r="C3" t="s">
         <v>12</v>
       </c>
@@ -2334,10 +2340,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="51"/>
+      <c r="B10" s="50"/>
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -2464,10 +2470,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="51"/>
+      <c r="B19" s="50"/>
       <c r="C19" t="s">
         <v>12</v>
       </c>
@@ -2481,10 +2487,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="51"/>
+      <c r="B21" s="50"/>
       <c r="C21" t="s">
         <v>111</v>
       </c>
@@ -2505,11 +2511,11 @@
       <c r="H22" t="s">
         <v>253</v>
       </c>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
@@ -2527,17 +2533,17 @@
       <c r="H23" t="s">
         <v>254</v>
       </c>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="51"/>
+      <c r="B24" s="50"/>
       <c r="C24" t="s">
         <v>111</v>
       </c>
@@ -2605,10 +2611,10 @@
       <c r="M27" s="15"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="51"/>
+      <c r="B28" s="50"/>
       <c r="C28" t="s">
         <v>111</v>
       </c>
@@ -2729,10 +2735,10 @@
       <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="51"/>
+      <c r="B34" s="50"/>
       <c r="C34" t="s">
         <v>12</v>
       </c>
@@ -2896,10 +2902,10 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="51"/>
+      <c r="B45" s="50"/>
       <c r="C45" t="s">
         <v>111</v>
       </c>
@@ -2980,10 +2986,10 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="51" t="s">
+      <c r="A49" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="51"/>
+      <c r="B49" s="50"/>
       <c r="C49" t="s">
         <v>111</v>
       </c>
@@ -3057,10 +3063,10 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="51" t="s">
+      <c r="A54" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="51"/>
+      <c r="B54" s="50"/>
       <c r="C54" t="s">
         <v>19</v>
       </c>
@@ -3184,10 +3190,10 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="51" t="s">
+      <c r="A63" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="B63" s="51"/>
+      <c r="B63" s="50"/>
       <c r="C63" t="s">
         <v>12</v>
       </c>
@@ -3337,10 +3343,10 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="51" t="s">
+      <c r="A73" s="50" t="s">
         <v>273</v>
       </c>
-      <c r="B73" s="51"/>
+      <c r="B73" s="50"/>
       <c r="C73" s="16" t="s">
         <v>12</v>
       </c>
@@ -3652,6 +3658,9 @@
       <c r="D95" t="b">
         <v>1</v>
       </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
       <c r="G95" t="s">
         <v>177</v>
       </c>
@@ -3669,6 +3678,9 @@
       <c r="D96" t="b">
         <v>1</v>
       </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
       <c r="G96" t="s">
         <v>178</v>
       </c>
@@ -3686,6 +3698,9 @@
       <c r="D97" t="b">
         <v>1</v>
       </c>
+      <c r="E97">
+        <v>2</v>
+      </c>
       <c r="G97" t="s">
         <v>179</v>
       </c>
@@ -3871,10 +3886,10 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="51" t="s">
+      <c r="A110" s="50" t="s">
         <v>261</v>
       </c>
-      <c r="B110" s="51"/>
+      <c r="B110" s="50"/>
       <c r="C110" t="s">
         <v>12</v>
       </c>
@@ -4159,10 +4174,10 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="51" t="s">
+      <c r="A129" s="50" t="s">
         <v>264</v>
       </c>
-      <c r="B129" s="51"/>
+      <c r="B129" s="50"/>
       <c r="C129" t="s">
         <v>111</v>
       </c>
@@ -4210,10 +4225,10 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A133" s="51" t="s">
+      <c r="A133" s="50" t="s">
         <v>256</v>
       </c>
-      <c r="B133" s="51"/>
+      <c r="B133" s="50"/>
       <c r="C133" t="s">
         <v>12</v>
       </c>
@@ -4231,10 +4246,10 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="51" t="s">
+      <c r="A135" s="50" t="s">
         <v>267</v>
       </c>
-      <c r="B135" s="51"/>
+      <c r="B135" s="50"/>
       <c r="C135" t="s">
         <v>12</v>
       </c>
@@ -4299,10 +4314,10 @@
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="51" t="s">
+      <c r="A140" s="50" t="s">
         <v>383</v>
       </c>
-      <c r="B140" s="51"/>
+      <c r="B140" s="50"/>
       <c r="C140" t="s">
         <v>19</v>
       </c>
@@ -4350,10 +4365,10 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="51" t="s">
+      <c r="A144" s="50" t="s">
         <v>380</v>
       </c>
-      <c r="B144" s="51"/>
+      <c r="B144" s="50"/>
       <c r="C144" t="s">
         <v>111</v>
       </c>
@@ -4390,10 +4405,10 @@
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A147" s="51" t="s">
+      <c r="A147" s="50" t="s">
         <v>444</v>
       </c>
-      <c r="B147" s="51"/>
+      <c r="B147" s="50"/>
       <c r="C147" t="s">
         <v>111</v>
       </c>
@@ -4446,10 +4461,10 @@
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A152" s="51" t="s">
+      <c r="A152" s="50" t="s">
         <v>263</v>
       </c>
-      <c r="B152" s="51"/>
+      <c r="B152" s="50"/>
       <c r="C152" t="s">
         <v>12</v>
       </c>
@@ -4559,19 +4574,22 @@
       <c r="C160" t="s">
         <v>313</v>
       </c>
+      <c r="F160" t="s">
+        <v>451</v>
+      </c>
       <c r="G160" t="s">
         <v>374</v>
       </c>
       <c r="H160" t="s">
         <v>376</v>
       </c>
-      <c r="I160" s="50" t="s">
+      <c r="I160" s="52" t="s">
         <v>379</v>
       </c>
-      <c r="J160" s="50"/>
-      <c r="K160" s="50"/>
-      <c r="L160" s="50"/>
-      <c r="M160" s="50"/>
+      <c r="J160" s="52"/>
+      <c r="K160" s="52"/>
+      <c r="L160" s="52"/>
+      <c r="M160" s="52"/>
     </row>
     <row r="161" spans="2:13" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
@@ -4580,19 +4598,22 @@
       <c r="C161" t="s">
         <v>53</v>
       </c>
+      <c r="F161" t="s">
+        <v>451</v>
+      </c>
       <c r="G161" t="s">
         <v>375</v>
       </c>
       <c r="H161" t="s">
         <v>377</v>
       </c>
-      <c r="I161" s="50" t="s">
+      <c r="I161" s="52" t="s">
         <v>378</v>
       </c>
-      <c r="J161" s="50"/>
-      <c r="K161" s="50"/>
-      <c r="L161" s="50"/>
-      <c r="M161" s="50"/>
+      <c r="J161" s="52"/>
+      <c r="K161" s="52"/>
+      <c r="L161" s="52"/>
+      <c r="M161" s="52"/>
     </row>
     <row r="162" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
@@ -4604,15 +4625,23 @@
       <c r="G162" t="s">
         <v>445</v>
       </c>
+      <c r="H162" t="s">
+        <v>452</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:M161" xr:uid="{A98571A1-046A-F843-AA6D-99F644BB2C36}"/>
   <mergeCells count="23">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="I161:M161"/>
+    <mergeCell ref="I160:M160"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A73:B73"/>
     <mergeCell ref="I22:M23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A110:B110"/>
@@ -4621,16 +4650,11 @@
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="I161:M161"/>
-    <mergeCell ref="I160:M160"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Agregando el modulo de validacion de permisos
</commit_message>
<xml_diff>
--- a/doc/schemas.xlsx
+++ b/doc/schemas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1560" windowWidth="31120" windowHeight="18660" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="32500" windowHeight="17420" activeTab="5" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Schemas" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Bloques" sheetId="4" r:id="rId3"/>
     <sheet name="RBAC" sheetId="2" r:id="rId4"/>
     <sheet name="GWT" sheetId="3" r:id="rId5"/>
+    <sheet name="Roles" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schemas!$A$2:$M$161</definedName>
@@ -30,8 +31,595 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Arturo Rodolfo Castro Loera</author>
+  </authors>
+  <commentList>
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{1F69AEAE-97B5-BA4A-81E7-7F3C5AA3424E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Se pueden hacer modificaciones, pero solo hasta antes de que comience el grupo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V8" authorId="0" shapeId="0" xr:uid="{8F7A413C-7351-2148-8474-31DB63A30AF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Puede crear grupos a nivel organizaci</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ón</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S9" authorId="0" shapeId="0" xr:uid="{65FAD601-4F81-DA41-B0A8-E042507B8CBC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Solo puede ver contenido de su propia orgUnit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T9" authorId="0" shapeId="0" xr:uid="{918FB9B7-235D-2C47-9869-BEBAB1D38608}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Su propio contenido</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U9" authorId="0" shapeId="0" xr:uid="{ED8D3FD3-E5AF-3841-91B9-831C5DD76BDB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Su propio contenido</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V10" authorId="0" shapeId="0" xr:uid="{3DC4F1F0-A84A-7044-9365-1C8A44FC2CB0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Puede crear grupos a nivel unidad organizacional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X10" authorId="0" shapeId="0" xr:uid="{D4C39FB6-BCD6-5A47-B7BB-9BDF05477153}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Solo puede modificar los que cre</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ó</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y10" authorId="0" shapeId="0" xr:uid="{8C8755F1-1991-D94F-A854-602420F8EAA1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Solo los que el instructor cre</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ó</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V11" authorId="0" shapeId="0" xr:uid="{2F8C6D5D-9B07-F44A-BF65-25E8FBE24B71}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Puede crear grupos a nivel unidad organizacional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X11" authorId="0" shapeId="0" xr:uid="{845835A2-0AD2-B646-8C5A-A504691ABB4F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>solo puede modificar los que cre</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ó</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y11" authorId="0" shapeId="0" xr:uid="{FF613EDD-B581-9E4E-A8ED-3C70DE6E5797}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>solo los que el supervisor cre</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ó</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N12" authorId="0" shapeId="0" xr:uid="{84690DDD-090E-784D-9B3B-56ABBFD8926A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Su propio usuario</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O12" authorId="0" shapeId="0" xr:uid="{3EAE670F-60D4-1C43-A022-D412AE6B1A49}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Su propio usuario</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P12" authorId="0" shapeId="0" xr:uid="{2A5A4AE9-22FE-3E4D-9744-E2312640815F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Rodolfo Castro Loera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Su propio usuario</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="474">
   <si>
     <t>Collections</t>
   </si>
@@ -1390,6 +1978,69 @@
   </si>
   <si>
     <t>Para controlar las fechas por bloque y sección</t>
+  </si>
+  <si>
+    <t>isAdmin</t>
+  </si>
+  <si>
+    <t>isBusiness</t>
+  </si>
+  <si>
+    <t>isOrg</t>
+  </si>
+  <si>
+    <t>isOrgContent</t>
+  </si>
+  <si>
+    <t>isAuthor</t>
+  </si>
+  <si>
+    <t>isInstructor</t>
+  </si>
+  <si>
+    <t>isSupervisor</t>
+  </si>
+  <si>
+    <t>Configurar reglas de precios y costos para grupos</t>
+  </si>
+  <si>
+    <t>Alumno</t>
+  </si>
+  <si>
+    <t>Contenido</t>
+  </si>
+  <si>
+    <t>Configurar Plataforma</t>
+  </si>
+  <si>
+    <t>Organizaciones</t>
+  </si>
+  <si>
+    <t>Crear</t>
+  </si>
+  <si>
+    <t>Ver</t>
+  </si>
+  <si>
+    <t>Modificar</t>
+  </si>
+  <si>
+    <t>Permisos</t>
+  </si>
+  <si>
+    <t>Unidades Org</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>Grupos</t>
+  </si>
+  <si>
+    <t>La creación se controla por el API</t>
+  </si>
+  <si>
+    <t>Usuario con privilegios</t>
   </si>
 </sst>
 </file>
@@ -1401,7 +2052,7 @@
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1479,8 +2130,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1553,8 +2217,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1705,12 +2381,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1829,24 +2514,91 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2188,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB6E249-7676-0040-9A74-86494BA4AA54}">
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E156" sqref="E156"/>
     </sheetView>
   </sheetViews>
@@ -2235,10 +2987,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="50"/>
+      <c r="B3" s="51"/>
       <c r="C3" t="s">
         <v>12</v>
       </c>
@@ -2340,10 +3092,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="50"/>
+      <c r="B10" s="51"/>
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -2470,10 +3222,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="50"/>
+      <c r="B19" s="51"/>
       <c r="C19" t="s">
         <v>12</v>
       </c>
@@ -2487,10 +3239,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="50"/>
+      <c r="B21" s="51"/>
       <c r="C21" t="s">
         <v>111</v>
       </c>
@@ -2511,11 +3263,11 @@
       <c r="H22" t="s">
         <v>253</v>
       </c>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
@@ -2533,17 +3285,17 @@
       <c r="H23" t="s">
         <v>254</v>
       </c>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="50"/>
+      <c r="B24" s="51"/>
       <c r="C24" t="s">
         <v>111</v>
       </c>
@@ -2611,10 +3363,10 @@
       <c r="M27" s="15"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="50"/>
+      <c r="B28" s="51"/>
       <c r="C28" t="s">
         <v>111</v>
       </c>
@@ -2735,10 +3487,10 @@
       <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="50" t="s">
+      <c r="A34" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="50"/>
+      <c r="B34" s="51"/>
       <c r="C34" t="s">
         <v>12</v>
       </c>
@@ -2902,10 +3654,10 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="50" t="s">
+      <c r="A45" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="50"/>
+      <c r="B45" s="51"/>
       <c r="C45" t="s">
         <v>111</v>
       </c>
@@ -2986,10 +3738,10 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="50" t="s">
+      <c r="A49" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="50"/>
+      <c r="B49" s="51"/>
       <c r="C49" t="s">
         <v>111</v>
       </c>
@@ -3063,10 +3815,10 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="50" t="s">
+      <c r="A54" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="50"/>
+      <c r="B54" s="51"/>
       <c r="C54" t="s">
         <v>19</v>
       </c>
@@ -3190,10 +3942,10 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="50" t="s">
+      <c r="A63" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="B63" s="50"/>
+      <c r="B63" s="51"/>
       <c r="C63" t="s">
         <v>12</v>
       </c>
@@ -3343,10 +4095,10 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="50" t="s">
+      <c r="A73" s="51" t="s">
         <v>273</v>
       </c>
-      <c r="B73" s="50"/>
+      <c r="B73" s="51"/>
       <c r="C73" s="16" t="s">
         <v>12</v>
       </c>
@@ -3886,10 +4638,10 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="50" t="s">
+      <c r="A110" s="51" t="s">
         <v>261</v>
       </c>
-      <c r="B110" s="50"/>
+      <c r="B110" s="51"/>
       <c r="C110" t="s">
         <v>12</v>
       </c>
@@ -4174,10 +4926,10 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="50" t="s">
+      <c r="A129" s="51" t="s">
         <v>264</v>
       </c>
-      <c r="B129" s="50"/>
+      <c r="B129" s="51"/>
       <c r="C129" t="s">
         <v>111</v>
       </c>
@@ -4225,10 +4977,10 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A133" s="50" t="s">
+      <c r="A133" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="B133" s="50"/>
+      <c r="B133" s="51"/>
       <c r="C133" t="s">
         <v>12</v>
       </c>
@@ -4246,10 +4998,10 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="50" t="s">
+      <c r="A135" s="51" t="s">
         <v>267</v>
       </c>
-      <c r="B135" s="50"/>
+      <c r="B135" s="51"/>
       <c r="C135" t="s">
         <v>12</v>
       </c>
@@ -4314,10 +5066,10 @@
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="50" t="s">
+      <c r="A140" s="51" t="s">
         <v>383</v>
       </c>
-      <c r="B140" s="50"/>
+      <c r="B140" s="51"/>
       <c r="C140" t="s">
         <v>19</v>
       </c>
@@ -4365,10 +5117,10 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="50" t="s">
+      <c r="A144" s="51" t="s">
         <v>380</v>
       </c>
-      <c r="B144" s="50"/>
+      <c r="B144" s="51"/>
       <c r="C144" t="s">
         <v>111</v>
       </c>
@@ -4405,10 +5157,10 @@
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A147" s="50" t="s">
+      <c r="A147" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="B147" s="50"/>
+      <c r="B147" s="51"/>
       <c r="C147" t="s">
         <v>111</v>
       </c>
@@ -4461,10 +5213,10 @@
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A152" s="50" t="s">
+      <c r="A152" s="51" t="s">
         <v>263</v>
       </c>
-      <c r="B152" s="50"/>
+      <c r="B152" s="51"/>
       <c r="C152" t="s">
         <v>12</v>
       </c>
@@ -4583,13 +5335,13 @@
       <c r="H160" t="s">
         <v>376</v>
       </c>
-      <c r="I160" s="52" t="s">
+      <c r="I160" s="50" t="s">
         <v>379</v>
       </c>
-      <c r="J160" s="52"/>
-      <c r="K160" s="52"/>
-      <c r="L160" s="52"/>
-      <c r="M160" s="52"/>
+      <c r="J160" s="50"/>
+      <c r="K160" s="50"/>
+      <c r="L160" s="50"/>
+      <c r="M160" s="50"/>
     </row>
     <row r="161" spans="2:13" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
@@ -4607,13 +5359,13 @@
       <c r="H161" t="s">
         <v>377</v>
       </c>
-      <c r="I161" s="52" t="s">
+      <c r="I161" s="50" t="s">
         <v>378</v>
       </c>
-      <c r="J161" s="52"/>
-      <c r="K161" s="52"/>
-      <c r="L161" s="52"/>
-      <c r="M161" s="52"/>
+      <c r="J161" s="50"/>
+      <c r="K161" s="50"/>
+      <c r="L161" s="50"/>
+      <c r="M161" s="50"/>
     </row>
     <row r="162" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
@@ -4632,16 +5384,11 @@
   </sheetData>
   <autoFilter ref="A2:M161" xr:uid="{A98571A1-046A-F843-AA6D-99F644BB2C36}"/>
   <mergeCells count="23">
-    <mergeCell ref="I161:M161"/>
-    <mergeCell ref="I160:M160"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="I22:M23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A110:B110"/>
@@ -4650,11 +5397,16 @@
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="I161:M161"/>
+    <mergeCell ref="I160:M160"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A147:B147"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5317,7 +6069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12457892-A860-024C-BFC8-6E106FE379AF}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -5852,10 +6604,10 @@
     <mergeCell ref="S7:S14"/>
   </mergeCells>
   <conditionalFormatting sqref="S16">
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
       <formula>$S$16&gt;=$B$3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>$S$16&lt;$B$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5872,4 +6624,612 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DDB1C7-C872-B544-A08C-E0F0B1219F70}">
+  <dimension ref="B1:Y13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" customWidth="1"/>
+    <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="12.1640625" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:25" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="52" t="s">
+        <v>463</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>460</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>464</v>
+      </c>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="59" t="s">
+        <v>469</v>
+      </c>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="61" t="s">
+        <v>462</v>
+      </c>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="54" t="s">
+        <v>471</v>
+      </c>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+    </row>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="55" t="s">
+        <v>465</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>466</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>467</v>
+      </c>
+      <c r="I2" s="58" t="s">
+        <v>468</v>
+      </c>
+      <c r="J2" s="55" t="s">
+        <v>465</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>466</v>
+      </c>
+      <c r="L2" s="57" t="s">
+        <v>467</v>
+      </c>
+      <c r="M2" s="58" t="s">
+        <v>468</v>
+      </c>
+      <c r="N2" s="55" t="s">
+        <v>465</v>
+      </c>
+      <c r="O2" s="56" t="s">
+        <v>466</v>
+      </c>
+      <c r="P2" s="57" t="s">
+        <v>467</v>
+      </c>
+      <c r="Q2" s="58" t="s">
+        <v>468</v>
+      </c>
+      <c r="R2" s="55" t="s">
+        <v>465</v>
+      </c>
+      <c r="S2" s="56" t="s">
+        <v>466</v>
+      </c>
+      <c r="T2" s="57" t="s">
+        <v>467</v>
+      </c>
+      <c r="U2" s="58" t="s">
+        <v>468</v>
+      </c>
+      <c r="V2" s="55" t="s">
+        <v>465</v>
+      </c>
+      <c r="W2" s="56" t="s">
+        <v>466</v>
+      </c>
+      <c r="X2" s="57" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y2" s="58" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B3" s="62" t="s">
+        <v>473</v>
+      </c>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="V3" s="62"/>
+      <c r="W3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="X3" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="64"/>
+      <c r="V4" s="64"/>
+      <c r="W4" s="64"/>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B5" s="63" t="s">
+        <v>453</v>
+      </c>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+      <c r="X5" s="63"/>
+      <c r="Y5" s="63"/>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B6" s="63" t="s">
+        <v>454</v>
+      </c>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" s="63"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="63"/>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B7" s="63" t="s">
+        <v>455</v>
+      </c>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="63"/>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B8" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="V8" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="W8" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="X8" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B9" s="63" t="s">
+        <v>457</v>
+      </c>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="U9" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="63"/>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B10" s="63" t="s">
+        <v>458</v>
+      </c>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="W10" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="X10" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B11" s="63" t="s">
+        <v>459</v>
+      </c>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="W11" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="X11" s="63" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B12" s="62" t="s">
+        <v>461</v>
+      </c>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="P12" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="62"/>
+      <c r="T12" s="62"/>
+      <c r="U12" s="62"/>
+      <c r="V12" s="62"/>
+      <c r="W12" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="X12" s="62"/>
+      <c r="Y12" s="62"/>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>472</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="R1:U1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D5:AQ12">
+    <cfRule type="expression" dxfId="3" priority="7" stopIfTrue="1">
+      <formula>D5=FALSE</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>D5=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:AQ4">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>D3=FALSE</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>D3=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agregando comentarios al archivo de schemas.xlsx
</commit_message>
<xml_diff>
--- a/doc/schemas.xlsx
+++ b/doc/schemas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -99,16 +99,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Puede crear grupos a nivel organizaci</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ón</t>
+          <t>Puede crear grupos a nivel organización</t>
         </r>
       </text>
     </comment>
@@ -345,16 +336,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Solo los que el instructor cre</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ó</t>
+          <t>Solo los que el instructor creó</t>
         </r>
       </text>
     </comment>
@@ -482,16 +464,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>solo los que el supervisor cre</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ó</t>
+          <t>solo los que el supervisor creó</t>
         </r>
       </text>
     </comment>
@@ -619,7 +592,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="487">
   <si>
     <t>Collections</t>
   </si>
@@ -2007,9 +1980,6 @@
     <t>Alumno</t>
   </si>
   <si>
-    <t>Contenido</t>
-  </si>
-  <si>
     <t>Configurar Plataforma</t>
   </si>
   <si>
@@ -2041,6 +2011,48 @@
   </si>
   <si>
     <t>Usuario con privilegios</t>
+  </si>
+  <si>
+    <t>Contenido / Cursos</t>
+  </si>
+  <si>
+    <t>Usuario_Conalep</t>
+  </si>
+  <si>
+    <t>CONALEP</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Visitante</t>
+  </si>
+  <si>
+    <t>Usuario_CETEC</t>
+  </si>
+  <si>
+    <t>CETEC</t>
+  </si>
+  <si>
+    <t>Tipo de usuario</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>Que puede ver el usuario</t>
+  </si>
+  <si>
+    <t>usuario_x</t>
+  </si>
+  <si>
+    <t>usuario_y</t>
+  </si>
+  <si>
+    <t>usuario_public</t>
+  </si>
+  <si>
+    <t>usuario_conalep</t>
   </si>
 </sst>
 </file>
@@ -2514,6 +2526,21 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2526,20 +2553,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2547,12 +2565,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2987,10 +2999,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="51"/>
+      <c r="B3" s="58"/>
       <c r="C3" t="s">
         <v>12</v>
       </c>
@@ -3092,10 +3104,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="51"/>
+      <c r="B10" s="58"/>
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -3222,10 +3234,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="51"/>
+      <c r="B19" s="58"/>
       <c r="C19" t="s">
         <v>12</v>
       </c>
@@ -3239,10 +3251,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="51"/>
+      <c r="B21" s="58"/>
       <c r="C21" t="s">
         <v>111</v>
       </c>
@@ -3263,11 +3275,11 @@
       <c r="H22" t="s">
         <v>253</v>
       </c>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
@@ -3285,17 +3297,17 @@
       <c r="H23" t="s">
         <v>254</v>
       </c>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="51"/>
+      <c r="B24" s="58"/>
       <c r="C24" t="s">
         <v>111</v>
       </c>
@@ -3363,10 +3375,10 @@
       <c r="M27" s="15"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="51"/>
+      <c r="B28" s="58"/>
       <c r="C28" t="s">
         <v>111</v>
       </c>
@@ -3487,10 +3499,10 @@
       <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="51"/>
+      <c r="B34" s="58"/>
       <c r="C34" t="s">
         <v>12</v>
       </c>
@@ -3654,10 +3666,10 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="51"/>
+      <c r="B45" s="58"/>
       <c r="C45" t="s">
         <v>111</v>
       </c>
@@ -3738,10 +3750,10 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="51" t="s">
+      <c r="A49" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="51"/>
+      <c r="B49" s="58"/>
       <c r="C49" t="s">
         <v>111</v>
       </c>
@@ -3815,10 +3827,10 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="51" t="s">
+      <c r="A54" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="51"/>
+      <c r="B54" s="58"/>
       <c r="C54" t="s">
         <v>19</v>
       </c>
@@ -3942,10 +3954,10 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="51" t="s">
+      <c r="A63" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="B63" s="51"/>
+      <c r="B63" s="58"/>
       <c r="C63" t="s">
         <v>12</v>
       </c>
@@ -4095,10 +4107,10 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="51" t="s">
+      <c r="A73" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="B73" s="51"/>
+      <c r="B73" s="58"/>
       <c r="C73" s="16" t="s">
         <v>12</v>
       </c>
@@ -4638,10 +4650,10 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="51" t="s">
+      <c r="A110" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="B110" s="51"/>
+      <c r="B110" s="58"/>
       <c r="C110" t="s">
         <v>12</v>
       </c>
@@ -4926,10 +4938,10 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="51" t="s">
+      <c r="A129" s="58" t="s">
         <v>264</v>
       </c>
-      <c r="B129" s="51"/>
+      <c r="B129" s="58"/>
       <c r="C129" t="s">
         <v>111</v>
       </c>
@@ -4977,10 +4989,10 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A133" s="51" t="s">
+      <c r="A133" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="B133" s="51"/>
+      <c r="B133" s="58"/>
       <c r="C133" t="s">
         <v>12</v>
       </c>
@@ -4998,10 +5010,10 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="51" t="s">
+      <c r="A135" s="58" t="s">
         <v>267</v>
       </c>
-      <c r="B135" s="51"/>
+      <c r="B135" s="58"/>
       <c r="C135" t="s">
         <v>12</v>
       </c>
@@ -5066,10 +5078,10 @@
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="51" t="s">
+      <c r="A140" s="58" t="s">
         <v>383</v>
       </c>
-      <c r="B140" s="51"/>
+      <c r="B140" s="58"/>
       <c r="C140" t="s">
         <v>19</v>
       </c>
@@ -5117,10 +5129,10 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="51" t="s">
+      <c r="A144" s="58" t="s">
         <v>380</v>
       </c>
-      <c r="B144" s="51"/>
+      <c r="B144" s="58"/>
       <c r="C144" t="s">
         <v>111</v>
       </c>
@@ -5157,10 +5169,10 @@
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A147" s="51" t="s">
+      <c r="A147" s="58" t="s">
         <v>444</v>
       </c>
-      <c r="B147" s="51"/>
+      <c r="B147" s="58"/>
       <c r="C147" t="s">
         <v>111</v>
       </c>
@@ -5213,10 +5225,10 @@
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A152" s="51" t="s">
+      <c r="A152" s="58" t="s">
         <v>263</v>
       </c>
-      <c r="B152" s="51"/>
+      <c r="B152" s="58"/>
       <c r="C152" t="s">
         <v>12</v>
       </c>
@@ -5335,13 +5347,13 @@
       <c r="H160" t="s">
         <v>376</v>
       </c>
-      <c r="I160" s="50" t="s">
+      <c r="I160" s="57" t="s">
         <v>379</v>
       </c>
-      <c r="J160" s="50"/>
-      <c r="K160" s="50"/>
-      <c r="L160" s="50"/>
-      <c r="M160" s="50"/>
+      <c r="J160" s="57"/>
+      <c r="K160" s="57"/>
+      <c r="L160" s="57"/>
+      <c r="M160" s="57"/>
     </row>
     <row r="161" spans="2:13" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
@@ -5359,13 +5371,13 @@
       <c r="H161" t="s">
         <v>377</v>
       </c>
-      <c r="I161" s="50" t="s">
+      <c r="I161" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="J161" s="50"/>
-      <c r="K161" s="50"/>
-      <c r="L161" s="50"/>
-      <c r="M161" s="50"/>
+      <c r="J161" s="57"/>
+      <c r="K161" s="57"/>
+      <c r="L161" s="57"/>
+      <c r="M161" s="57"/>
     </row>
     <row r="162" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
@@ -6131,7 +6143,7 @@
       <c r="R7" s="31">
         <v>4</v>
       </c>
-      <c r="S7" s="53" t="s">
+      <c r="S7" s="60" t="s">
         <v>340</v>
       </c>
     </row>
@@ -6190,7 +6202,7 @@
       <c r="R8" s="32">
         <v>0</v>
       </c>
-      <c r="S8" s="53"/>
+      <c r="S8" s="60"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -6247,7 +6259,7 @@
       <c r="R9" s="19">
         <v>0</v>
       </c>
-      <c r="S9" s="53"/>
+      <c r="S9" s="60"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
@@ -6304,7 +6316,7 @@
       <c r="R10" s="34">
         <v>0</v>
       </c>
-      <c r="S10" s="53"/>
+      <c r="S10" s="60"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -6339,7 +6351,7 @@
         <f>R9*R10*R15</f>
         <v>0</v>
       </c>
-      <c r="S11" s="53"/>
+      <c r="S11" s="60"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -6396,7 +6408,7 @@
       <c r="R12" s="19">
         <v>1</v>
       </c>
-      <c r="S12" s="53"/>
+      <c r="S12" s="60"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
@@ -6453,7 +6465,7 @@
       <c r="R13" s="34">
         <v>1</v>
       </c>
-      <c r="S13" s="53"/>
+      <c r="S13" s="60"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -6488,7 +6500,7 @@
         <f>R12*R13*R15</f>
         <v>0</v>
       </c>
-      <c r="S14" s="53"/>
+      <c r="S14" s="60"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -6628,13 +6640,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DDB1C7-C872-B544-A08C-E0F0B1219F70}">
-  <dimension ref="B1:Y13"/>
+  <dimension ref="B1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6649,8 +6661,9 @@
     <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.6640625" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5" customWidth="1"/>
     <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.1640625" customWidth="1"/>
     <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
@@ -6659,559 +6672,657 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="59" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>460</v>
+      </c>
+      <c r="F1" s="62" t="s">
         <v>463</v>
       </c>
-      <c r="E1" s="52" t="s">
-        <v>460</v>
-      </c>
-      <c r="F1" s="54" t="s">
-        <v>464</v>
-      </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="59" t="s">
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="63" t="s">
+        <v>468</v>
+      </c>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="64" t="s">
         <v>469</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="60" t="s">
-        <v>470</v>
-      </c>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
       <c r="R1" s="61" t="s">
-        <v>462</v>
+        <v>473</v>
       </c>
       <c r="S1" s="61"/>
       <c r="T1" s="61"/>
       <c r="U1" s="61"/>
-      <c r="V1" s="54" t="s">
-        <v>471</v>
-      </c>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
+      <c r="V1" s="62" t="s">
+        <v>470</v>
+      </c>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="55" t="s">
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="50" t="s">
+        <v>464</v>
+      </c>
+      <c r="G2" s="51" t="s">
         <v>465</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="H2" s="52" t="s">
         <v>466</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="I2" s="53" t="s">
         <v>467</v>
       </c>
-      <c r="I2" s="58" t="s">
-        <v>468</v>
-      </c>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="50" t="s">
+        <v>464</v>
+      </c>
+      <c r="K2" s="51" t="s">
         <v>465</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="L2" s="52" t="s">
         <v>466</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="M2" s="53" t="s">
         <v>467</v>
       </c>
-      <c r="M2" s="58" t="s">
-        <v>468</v>
-      </c>
-      <c r="N2" s="55" t="s">
+      <c r="N2" s="50" t="s">
+        <v>464</v>
+      </c>
+      <c r="O2" s="51" t="s">
         <v>465</v>
       </c>
-      <c r="O2" s="56" t="s">
+      <c r="P2" s="52" t="s">
         <v>466</v>
       </c>
-      <c r="P2" s="57" t="s">
+      <c r="Q2" s="53" t="s">
         <v>467</v>
       </c>
-      <c r="Q2" s="58" t="s">
-        <v>468</v>
-      </c>
-      <c r="R2" s="55" t="s">
+      <c r="R2" s="50" t="s">
+        <v>464</v>
+      </c>
+      <c r="S2" s="51" t="s">
         <v>465</v>
       </c>
-      <c r="S2" s="56" t="s">
+      <c r="T2" s="52" t="s">
         <v>466</v>
       </c>
-      <c r="T2" s="57" t="s">
+      <c r="U2" s="53" t="s">
         <v>467</v>
       </c>
-      <c r="U2" s="58" t="s">
-        <v>468</v>
-      </c>
-      <c r="V2" s="55" t="s">
+      <c r="V2" s="50" t="s">
+        <v>464</v>
+      </c>
+      <c r="W2" s="51" t="s">
         <v>465</v>
       </c>
-      <c r="W2" s="56" t="s">
+      <c r="X2" s="52" t="s">
         <v>466</v>
       </c>
-      <c r="X2" s="57" t="s">
+      <c r="Y2" s="53" t="s">
         <v>467</v>
       </c>
-      <c r="Y2" s="58" t="s">
-        <v>468</v>
-      </c>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B3" s="62" t="s">
-        <v>473</v>
-      </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="P3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="62"/>
-      <c r="S3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="T3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="U3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="V3" s="62"/>
-      <c r="W3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="X3" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="62" t="b">
+      <c r="B3" s="54" t="s">
+        <v>472</v>
+      </c>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="X3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="54" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="55" t="s">
         <v>453</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="N5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="O5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="P5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" s="63"/>
-      <c r="S5" s="63"/>
-      <c r="T5" s="63"/>
-      <c r="U5" s="63"/>
-      <c r="V5" s="63"/>
-      <c r="W5" s="63"/>
-      <c r="X5" s="63"/>
-      <c r="Y5" s="63"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5" s="55"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="55"/>
+      <c r="V5" s="55"/>
+      <c r="W5" s="55"/>
+      <c r="X5" s="55"/>
+      <c r="Y5" s="55"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="55" t="s">
         <v>454</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="63"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="U6" s="63"/>
-      <c r="V6" s="63"/>
-      <c r="W6" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="X6" s="63"/>
-      <c r="Y6" s="63"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55"/>
+      <c r="S6" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" s="55"/>
+      <c r="V6" s="55"/>
+      <c r="W6" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="X6" s="55"/>
+      <c r="Y6" s="55"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="55" t="s">
         <v>455</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="N7" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="O7" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="P7" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="R7" s="63"/>
-      <c r="S7" s="63"/>
-      <c r="T7" s="63"/>
-      <c r="U7" s="63"/>
-      <c r="V7" s="63"/>
-      <c r="W7" s="63"/>
-      <c r="X7" s="63"/>
-      <c r="Y7" s="63"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" s="55"/>
+      <c r="S7" s="55"/>
+      <c r="T7" s="55"/>
+      <c r="U7" s="55"/>
+      <c r="V7" s="55"/>
+      <c r="W7" s="55"/>
+      <c r="X7" s="55"/>
+      <c r="Y7" s="55"/>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="55" t="s">
         <v>456</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="L8" s="63"/>
-      <c r="M8" s="63"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="P8" s="63"/>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="63"/>
-      <c r="S8" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="T8" s="63"/>
-      <c r="U8" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="V8" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="W8" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="X8" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="63" t="b">
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="V8" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="W8" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="X8" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="55" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="55" t="s">
         <v>457</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="S9" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="T9" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="U9" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="V9" s="63"/>
-      <c r="W9" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="X9" s="63"/>
-      <c r="Y9" s="63"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="U9" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="V9" s="55"/>
+      <c r="W9" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="X9" s="55"/>
+      <c r="Y9" s="55"/>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="55" t="s">
         <v>458</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="63"/>
-      <c r="R10" s="63"/>
-      <c r="S10" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="T10" s="63"/>
-      <c r="U10" s="63"/>
-      <c r="V10" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="W10" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="X10" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="63" t="b">
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="55"/>
+      <c r="S10" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10" s="55"/>
+      <c r="U10" s="55"/>
+      <c r="V10" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="W10" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="X10" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="55" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="55" t="s">
         <v>459</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="T11" s="63"/>
-      <c r="U11" s="63"/>
-      <c r="V11" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="W11" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="X11" s="63" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="63" t="b">
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="55"/>
+      <c r="R11" s="55"/>
+      <c r="S11" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11" s="55"/>
+      <c r="U11" s="55"/>
+      <c r="V11" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="W11" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="X11" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="55" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="54" t="s">
         <v>461</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
-      <c r="K12" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="62"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="P12" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="62"/>
-      <c r="R12" s="62"/>
-      <c r="S12" s="62"/>
-      <c r="T12" s="62"/>
-      <c r="U12" s="62"/>
-      <c r="V12" s="62"/>
-      <c r="W12" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="X12" s="62"/>
-      <c r="Y12" s="62"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="P12" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="54"/>
+      <c r="T12" s="54"/>
+      <c r="U12" s="54"/>
+      <c r="V12" s="54"/>
+      <c r="W12" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="X12" s="54"/>
+      <c r="Y12" s="54"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>472</v>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" ht="48" x14ac:dyDescent="0.2">
+      <c r="P14" t="s">
+        <v>480</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>481</v>
+      </c>
+      <c r="R14" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="S14" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="P16" t="s">
+        <v>477</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>85</v>
+      </c>
+      <c r="R16" t="s">
+        <v>85</v>
+      </c>
+      <c r="S16" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="17" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P17" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>475</v>
+      </c>
+      <c r="R17" t="s">
+        <v>475</v>
+      </c>
+      <c r="S17" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="18" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P18" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>85</v>
+      </c>
+      <c r="R18" t="s">
+        <v>85</v>
+      </c>
+      <c r="S18" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="19" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P19" t="s">
+        <v>478</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>479</v>
+      </c>
+      <c r="R19" t="s">
+        <v>479</v>
+      </c>
+      <c r="S19" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="20" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P20" t="s">
+        <v>478</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>85</v>
+      </c>
+      <c r="R20" t="s">
+        <v>85</v>
+      </c>
+      <c r="S20" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="21" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P21" t="s">
+        <v>477</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>475</v>
+      </c>
+      <c r="R21" t="s">
+        <v>475</v>
+      </c>
+      <c r="S21" t="s">
+        <v>486</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="R1:U1"/>
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:AQ12">
     <cfRule type="expression" dxfId="3" priority="7" stopIfTrue="1">

</xml_diff>

<commit_message>
Agregando API para cargar de bloques
</commit_message>
<xml_diff>
--- a/doc/schemas.xlsx
+++ b/doc/schemas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10124"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="32500" windowHeight="17420" activeTab="5" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="32500" windowHeight="17420" activeTab="6" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Schemas" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="RBAC" sheetId="2" r:id="rId4"/>
     <sheet name="GWT" sheetId="3" r:id="rId5"/>
     <sheet name="Roles" sheetId="6" r:id="rId6"/>
+    <sheet name="Error Message Catalog" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schemas!$A$2:$M$161</definedName>
@@ -592,7 +593,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="492">
   <si>
     <t>Collections</t>
   </si>
@@ -2053,6 +2054,21 @@
   </si>
   <si>
     <t>usuario_conalep</t>
+  </si>
+  <si>
+    <t>Plataforma / Sistema</t>
+  </si>
+  <si>
+    <t>Sistema</t>
+  </si>
+  <si>
+    <t>Errores de roles</t>
+  </si>
+  <si>
+    <t>Autenticación</t>
+  </si>
+  <si>
+    <t>Error Message Catalog</t>
   </si>
 </sst>
 </file>
@@ -2541,14 +2557,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2999,10 +3015,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="58"/>
       <c r="C3" t="s">
         <v>12</v>
       </c>
@@ -3104,10 +3120,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="57"/>
+      <c r="B10" s="58"/>
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -3234,10 +3250,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="57"/>
+      <c r="B19" s="58"/>
       <c r="C19" t="s">
         <v>12</v>
       </c>
@@ -3251,10 +3267,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="57"/>
+      <c r="B21" s="58"/>
       <c r="C21" t="s">
         <v>111</v>
       </c>
@@ -3275,11 +3291,11 @@
       <c r="H22" t="s">
         <v>253</v>
       </c>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="58"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
@@ -3297,17 +3313,17 @@
       <c r="H23" t="s">
         <v>254</v>
       </c>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="58"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="57" t="s">
+      <c r="A24" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="57"/>
+      <c r="B24" s="58"/>
       <c r="C24" t="s">
         <v>111</v>
       </c>
@@ -3375,10 +3391,10 @@
       <c r="M27" s="15"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="57"/>
+      <c r="B28" s="58"/>
       <c r="C28" t="s">
         <v>111</v>
       </c>
@@ -3499,10 +3515,10 @@
       <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="57" t="s">
+      <c r="A34" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="57"/>
+      <c r="B34" s="58"/>
       <c r="C34" t="s">
         <v>12</v>
       </c>
@@ -3666,10 +3682,10 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="57" t="s">
+      <c r="A45" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="57"/>
+      <c r="B45" s="58"/>
       <c r="C45" t="s">
         <v>111</v>
       </c>
@@ -3750,10 +3766,10 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="57" t="s">
+      <c r="A49" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="57"/>
+      <c r="B49" s="58"/>
       <c r="C49" t="s">
         <v>111</v>
       </c>
@@ -3827,10 +3843,10 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="57" t="s">
+      <c r="A54" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="57"/>
+      <c r="B54" s="58"/>
       <c r="C54" t="s">
         <v>19</v>
       </c>
@@ -3954,10 +3970,10 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="57" t="s">
+      <c r="A63" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="B63" s="57"/>
+      <c r="B63" s="58"/>
       <c r="C63" t="s">
         <v>12</v>
       </c>
@@ -4107,10 +4123,10 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="57" t="s">
+      <c r="A73" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="B73" s="57"/>
+      <c r="B73" s="58"/>
       <c r="C73" s="16" t="s">
         <v>12</v>
       </c>
@@ -4650,10 +4666,10 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="57" t="s">
+      <c r="A110" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="B110" s="57"/>
+      <c r="B110" s="58"/>
       <c r="C110" t="s">
         <v>12</v>
       </c>
@@ -4938,10 +4954,10 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="57" t="s">
+      <c r="A129" s="58" t="s">
         <v>264</v>
       </c>
-      <c r="B129" s="57"/>
+      <c r="B129" s="58"/>
       <c r="C129" t="s">
         <v>111</v>
       </c>
@@ -4989,10 +5005,10 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A133" s="57" t="s">
+      <c r="A133" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="B133" s="57"/>
+      <c r="B133" s="58"/>
       <c r="C133" t="s">
         <v>12</v>
       </c>
@@ -5010,10 +5026,10 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="57" t="s">
+      <c r="A135" s="58" t="s">
         <v>267</v>
       </c>
-      <c r="B135" s="57"/>
+      <c r="B135" s="58"/>
       <c r="C135" t="s">
         <v>12</v>
       </c>
@@ -5078,10 +5094,10 @@
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="57" t="s">
+      <c r="A140" s="58" t="s">
         <v>383</v>
       </c>
-      <c r="B140" s="57"/>
+      <c r="B140" s="58"/>
       <c r="C140" t="s">
         <v>19</v>
       </c>
@@ -5129,10 +5145,10 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="57" t="s">
+      <c r="A144" s="58" t="s">
         <v>380</v>
       </c>
-      <c r="B144" s="57"/>
+      <c r="B144" s="58"/>
       <c r="C144" t="s">
         <v>111</v>
       </c>
@@ -5169,10 +5185,10 @@
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A147" s="57" t="s">
+      <c r="A147" s="58" t="s">
         <v>444</v>
       </c>
-      <c r="B147" s="57"/>
+      <c r="B147" s="58"/>
       <c r="C147" t="s">
         <v>111</v>
       </c>
@@ -5225,10 +5241,10 @@
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A152" s="57" t="s">
+      <c r="A152" s="58" t="s">
         <v>263</v>
       </c>
-      <c r="B152" s="57"/>
+      <c r="B152" s="58"/>
       <c r="C152" t="s">
         <v>12</v>
       </c>
@@ -5347,13 +5363,13 @@
       <c r="H160" t="s">
         <v>376</v>
       </c>
-      <c r="I160" s="59" t="s">
+      <c r="I160" s="57" t="s">
         <v>379</v>
       </c>
-      <c r="J160" s="59"/>
-      <c r="K160" s="59"/>
-      <c r="L160" s="59"/>
-      <c r="M160" s="59"/>
+      <c r="J160" s="57"/>
+      <c r="K160" s="57"/>
+      <c r="L160" s="57"/>
+      <c r="M160" s="57"/>
     </row>
     <row r="161" spans="2:13" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
@@ -5371,13 +5387,13 @@
       <c r="H161" t="s">
         <v>377</v>
       </c>
-      <c r="I161" s="59" t="s">
+      <c r="I161" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="J161" s="59"/>
-      <c r="K161" s="59"/>
-      <c r="L161" s="59"/>
-      <c r="M161" s="59"/>
+      <c r="J161" s="57"/>
+      <c r="K161" s="57"/>
+      <c r="L161" s="57"/>
+      <c r="M161" s="57"/>
     </row>
     <row r="162" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
@@ -5396,16 +5412,11 @@
   </sheetData>
   <autoFilter ref="A2:M161" xr:uid="{A98571A1-046A-F843-AA6D-99F644BB2C36}"/>
   <mergeCells count="23">
-    <mergeCell ref="I161:M161"/>
-    <mergeCell ref="I160:M160"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="I22:M23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A110:B110"/>
@@ -5414,11 +5425,16 @@
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="I161:M161"/>
+    <mergeCell ref="I160:M160"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A147:B147"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6642,7 +6658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DDB1C7-C872-B544-A08C-E0F0B1219F70}">
   <dimension ref="B1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
+    <sheetView zoomScale="174" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -6672,10 +6688,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="59" t="s">
         <v>462</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="59" t="s">
         <v>460</v>
       </c>
       <c r="F1" s="62" t="s">
@@ -6710,8 +6726,8 @@
       <c r="Y1" s="62"/>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
       <c r="F2" s="50" t="s">
         <v>464</v>
       </c>
@@ -7343,4 +7359,178 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC262E40-55B7-BC40-AE6A-332ED163D2AE}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="36">
+        <v>0</v>
+      </c>
+      <c r="B3" s="36">
+        <v>999</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>487</v>
+      </c>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>199</v>
+      </c>
+      <c r="C5" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>200</v>
+      </c>
+      <c r="B6">
+        <v>299</v>
+      </c>
+      <c r="C6" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="36">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="36">
+        <v>1999</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>489</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8">
+        <v>1999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2000</v>
+      </c>
+      <c r="B9">
+        <v>2999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3000</v>
+      </c>
+      <c r="B10">
+        <v>3999</v>
+      </c>
+      <c r="C10" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4000</v>
+      </c>
+      <c r="B11">
+        <v>4999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5000</v>
+      </c>
+      <c r="B12">
+        <v>5999</v>
+      </c>
+      <c r="C12" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6000</v>
+      </c>
+      <c r="B13">
+        <v>6999</v>
+      </c>
+      <c r="C13" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7000</v>
+      </c>
+      <c r="B14">
+        <v>7999</v>
+      </c>
+      <c r="C14" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>8000</v>
+      </c>
+      <c r="B15">
+        <v>8999</v>
+      </c>
+      <c r="C15" t="s">
+        <v>461</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agregando APIs para gestionar contenido
</commit_message>
<xml_diff>
--- a/doc/schemas.xlsx
+++ b/doc/schemas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10124"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="32500" windowHeight="17420" activeTab="6" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
+    <workbookView xWindow="1100" yWindow="680" windowWidth="32500" windowHeight="17420" activeTab="4" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Schemas" sheetId="1" r:id="rId1"/>
@@ -2969,7 +2969,7 @@
   <dimension ref="A1:M162"/>
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E156" sqref="E156"/>
     </sheetView>
   </sheetViews>
@@ -6097,8 +6097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12457892-A860-024C-BFC8-6E106FE379AF}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7365,7 +7365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC262E40-55B7-BC40-AE6A-332ED163D2AE}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrigiendo APIs y esquema de discusión
</commit_message>
<xml_diff>
--- a/doc/schemas.xlsx
+++ b/doc/schemas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10221"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Arturo/aclprojects/alumno/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2EA504-8C63-BC4E-BBD2-B928D1B6C246}" xr6:coauthVersionLast="30" xr6:coauthVersionMax="30" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543085CE-DCD4-8640-8A1F-B7A751C91C0C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="2500" windowWidth="32500" windowHeight="11780" activeTab="6" xr2:uid="{C53DE95F-88B2-1C4D-8A7D-A342AE2033F7}"/>
   </bookViews>
@@ -595,7 +595,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="523">
   <si>
     <t>Collections</t>
   </si>
@@ -2136,9 +2136,6 @@
     <t>titulo de la discusión</t>
   </si>
   <si>
-    <t>Discusión</t>
-  </si>
-  <si>
     <t>discussion</t>
   </si>
   <si>
@@ -2164,6 +2161,9 @@
   </si>
   <si>
     <t>["discussion","comment","reply"]</t>
+  </si>
+  <si>
+    <t>Discusión/Pregunta</t>
   </si>
 </sst>
 </file>
@@ -2652,14 +2652,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3113,10 +3113,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="58"/>
       <c r="C3" t="s">
         <v>12</v>
       </c>
@@ -3218,10 +3218,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="57"/>
+      <c r="B10" s="58"/>
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -3348,10 +3348,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="57"/>
+      <c r="B19" s="58"/>
       <c r="C19" t="s">
         <v>12</v>
       </c>
@@ -3365,10 +3365,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="57"/>
+      <c r="B21" s="58"/>
       <c r="C21" t="s">
         <v>111</v>
       </c>
@@ -3389,11 +3389,11 @@
       <c r="H22" t="s">
         <v>253</v>
       </c>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="58"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
@@ -3411,17 +3411,17 @@
       <c r="H23" t="s">
         <v>254</v>
       </c>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="58"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="57" t="s">
+      <c r="A24" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="57"/>
+      <c r="B24" s="58"/>
       <c r="C24" t="s">
         <v>111</v>
       </c>
@@ -3489,10 +3489,10 @@
       <c r="M27" s="15"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="57"/>
+      <c r="B28" s="58"/>
       <c r="C28" t="s">
         <v>111</v>
       </c>
@@ -3613,10 +3613,10 @@
       <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="57" t="s">
+      <c r="A34" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="57"/>
+      <c r="B34" s="58"/>
       <c r="C34" t="s">
         <v>12</v>
       </c>
@@ -3780,10 +3780,10 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="57" t="s">
+      <c r="A45" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="57"/>
+      <c r="B45" s="58"/>
       <c r="C45" t="s">
         <v>111</v>
       </c>
@@ -3864,10 +3864,10 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="57" t="s">
+      <c r="A49" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="57"/>
+      <c r="B49" s="58"/>
       <c r="C49" t="s">
         <v>111</v>
       </c>
@@ -3941,10 +3941,10 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="57" t="s">
+      <c r="A54" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="57"/>
+      <c r="B54" s="58"/>
       <c r="C54" t="s">
         <v>19</v>
       </c>
@@ -4068,10 +4068,10 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="57" t="s">
+      <c r="A63" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="B63" s="57"/>
+      <c r="B63" s="58"/>
       <c r="C63" t="s">
         <v>12</v>
       </c>
@@ -4221,10 +4221,10 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="57" t="s">
+      <c r="A73" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="B73" s="57"/>
+      <c r="B73" s="58"/>
       <c r="C73" s="16" t="s">
         <v>12</v>
       </c>
@@ -4764,10 +4764,10 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="57" t="s">
+      <c r="A110" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="B110" s="57"/>
+      <c r="B110" s="58"/>
       <c r="C110" t="s">
         <v>12</v>
       </c>
@@ -5052,10 +5052,10 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="57" t="s">
+      <c r="A129" s="58" t="s">
         <v>264</v>
       </c>
-      <c r="B129" s="57"/>
+      <c r="B129" s="58"/>
       <c r="C129" t="s">
         <v>111</v>
       </c>
@@ -5103,10 +5103,10 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A133" s="57" t="s">
+      <c r="A133" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="B133" s="57"/>
+      <c r="B133" s="58"/>
       <c r="C133" t="s">
         <v>12</v>
       </c>
@@ -5124,10 +5124,10 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="57" t="s">
+      <c r="A135" s="58" t="s">
         <v>267</v>
       </c>
-      <c r="B135" s="57"/>
+      <c r="B135" s="58"/>
       <c r="C135" t="s">
         <v>12</v>
       </c>
@@ -5192,10 +5192,10 @@
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="57" t="s">
+      <c r="A140" s="58" t="s">
         <v>383</v>
       </c>
-      <c r="B140" s="57"/>
+      <c r="B140" s="58"/>
       <c r="C140" t="s">
         <v>19</v>
       </c>
@@ -5243,10 +5243,10 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="57" t="s">
+      <c r="A144" s="58" t="s">
         <v>380</v>
       </c>
-      <c r="B144" s="57"/>
+      <c r="B144" s="58"/>
       <c r="C144" t="s">
         <v>111</v>
       </c>
@@ -5283,10 +5283,10 @@
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A147" s="57" t="s">
+      <c r="A147" s="58" t="s">
         <v>444</v>
       </c>
-      <c r="B147" s="57"/>
+      <c r="B147" s="58"/>
       <c r="C147" t="s">
         <v>111</v>
       </c>
@@ -5339,10 +5339,10 @@
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A152" s="57" t="s">
+      <c r="A152" s="58" t="s">
         <v>263</v>
       </c>
-      <c r="B152" s="57"/>
+      <c r="B152" s="58"/>
       <c r="C152" t="s">
         <v>12</v>
       </c>
@@ -5461,13 +5461,13 @@
       <c r="H160" t="s">
         <v>376</v>
       </c>
-      <c r="I160" s="59" t="s">
+      <c r="I160" s="57" t="s">
         <v>379</v>
       </c>
-      <c r="J160" s="59"/>
-      <c r="K160" s="59"/>
-      <c r="L160" s="59"/>
-      <c r="M160" s="59"/>
+      <c r="J160" s="57"/>
+      <c r="K160" s="57"/>
+      <c r="L160" s="57"/>
+      <c r="M160" s="57"/>
     </row>
     <row r="161" spans="2:13" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
@@ -5485,13 +5485,13 @@
       <c r="H161" t="s">
         <v>377</v>
       </c>
-      <c r="I161" s="59" t="s">
+      <c r="I161" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="J161" s="59"/>
-      <c r="K161" s="59"/>
-      <c r="L161" s="59"/>
-      <c r="M161" s="59"/>
+      <c r="J161" s="57"/>
+      <c r="K161" s="57"/>
+      <c r="L161" s="57"/>
+      <c r="M161" s="57"/>
     </row>
     <row r="162" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
@@ -5510,16 +5510,11 @@
   </sheetData>
   <autoFilter ref="A2:M161" xr:uid="{A98571A1-046A-F843-AA6D-99F644BB2C36}"/>
   <mergeCells count="23">
-    <mergeCell ref="I161:M161"/>
-    <mergeCell ref="I160:M160"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="I22:M23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A110:B110"/>
@@ -5528,11 +5523,16 @@
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="I161:M161"/>
+    <mergeCell ref="I160:M160"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A147:B147"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6786,10 +6786,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="59" t="s">
         <v>462</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="59" t="s">
         <v>460</v>
       </c>
       <c r="F1" s="62" t="s">
@@ -6824,8 +6824,8 @@
       <c r="Y1" s="62"/>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
       <c r="F2" s="50" t="s">
         <v>464</v>
       </c>
@@ -7461,10 +7461,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF278C6-F542-6A4C-AB15-30C5B6087111}">
-  <dimension ref="B2:U17"/>
+  <dimension ref="B2:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="274" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="274" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7497,7 +7497,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>513</v>
+        <v>522</v>
       </c>
       <c r="Q3" t="s">
         <v>503</v>
@@ -7505,14 +7505,11 @@
       <c r="R3" t="s">
         <v>43</v>
       </c>
+      <c r="S3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>522</v>
-      </c>
       <c r="L4">
         <v>2</v>
       </c>
@@ -7529,21 +7526,15 @@
         <v>497</v>
       </c>
       <c r="U4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>493</v>
-      </c>
-      <c r="F5" s="65" t="s">
-        <v>504</v>
-      </c>
       <c r="G5" t="s">
-        <v>514</v>
+        <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -7564,16 +7555,21 @@
         <v>505</v>
       </c>
       <c r="U5" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>493</v>
+      </c>
+      <c r="F6" s="65" t="s">
+        <v>504</v>
+      </c>
+      <c r="G6" t="s">
+        <v>513</v>
+      </c>
+      <c r="H6" t="s">
         <v>514</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="F6" s="65"/>
-      <c r="G6" t="s">
-        <v>505</v>
-      </c>
-      <c r="H6" t="s">
-        <v>521</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -7594,19 +7590,16 @@
         <v>505</v>
       </c>
       <c r="U6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>494</v>
-      </c>
       <c r="F7" s="65"/>
       <c r="G7" t="s">
-        <v>382</v>
+        <v>505</v>
       </c>
       <c r="H7" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="L7">
         <v>5</v>
@@ -7627,19 +7620,19 @@
         <v>505</v>
       </c>
       <c r="U7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F8" s="65"/>
       <c r="G8" t="s">
-        <v>278</v>
+        <v>382</v>
       </c>
       <c r="H8" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="L8">
         <v>6</v>
@@ -7647,14 +7640,14 @@
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F9" s="65"/>
       <c r="G9" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="H9" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="L9">
         <v>7</v>
@@ -7662,14 +7655,14 @@
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="F10" s="65"/>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>265</v>
       </c>
       <c r="H10" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="L10">
         <v>8</v>
@@ -7677,53 +7670,65 @@
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>508</v>
-      </c>
+        <v>509</v>
+      </c>
+      <c r="F11" s="65"/>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="H11" t="s">
-        <v>520</v>
-      </c>
-      <c r="L11">
-        <v>9</v>
+        <v>518</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
+        <v>508</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" t="s">
+        <v>519</v>
+      </c>
+      <c r="L12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
         <v>510</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>93</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>506</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="G13" t="s">
-        <v>498</v>
-      </c>
-      <c r="H13" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G14" t="s">
+        <v>498</v>
+      </c>
+      <c r="H14" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
         <v>257</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G17" t="s">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
         <v>511</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F5:F10"/>
+    <mergeCell ref="F6:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>